<commit_message>
Data updated till 7 Jan 11AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -22,6 +22,30 @@
     <author>Vijay</author>
   </authors>
   <commentList>
+    <comment ref="L48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1700-Cash
+2300-Digital
+2000-Digital</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AA56" authorId="0">
       <text>
         <r>
@@ -42,29 +66,6 @@
           <t xml:space="preserve">
 1500-Cash
 500-Digital</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L66" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t>Vijay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t xml:space="preserve">
-3000-Digital
-1000-Cash</t>
         </r>
       </text>
     </comment>
@@ -428,7 +429,7 @@
     <t>ROHIT SHOE STORE(661670729)</t>
   </si>
   <si>
-    <t>Indrijeet</t>
+    <t>INDRJEET KUMAR</t>
   </si>
   <si>
     <t>Dhewai</t>
@@ -520,11 +521,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -543,13 +544,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -565,8 +559,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,14 +608,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,9 +636,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,36 +645,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -674,7 +668,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -731,25 +732,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,31 +750,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,7 +774,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,13 +822,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,13 +888,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,37 +900,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -893,25 +912,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,6 +923,47 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -966,35 +1008,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1007,35 +1023,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1045,130 +1046,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1190,7 +1191,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1546,11 +1547,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G58" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L71" sqref="L71"/>
+      <selection pane="bottomRight" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1687,14 +1688,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>212900</v>
+        <v>266800</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>212900</v>
+        <v>266800</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1718,7 +1719,7 @@
       </c>
       <c r="L2" s="2">
         <f t="shared" ref="L2:AK2" si="0">SUM(L3:L120)</f>
-        <v>0</v>
+        <v>53900</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" si="0"/>
@@ -1911,7 +1912,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:10">
+    <row r="7" s="3" customFormat="1" spans="1:12">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1926,13 +1927,16 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>11000</v>
       </c>
       <c r="J7" s="11">
         <v>4000</v>
       </c>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:6">
+      <c r="L7" s="11">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:12">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1947,7 +1951,10 @@
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1" spans="1:11">
@@ -1992,7 +1999,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="1" spans="1:6">
+    <row r="11" s="3" customFormat="1" spans="1:12">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2010,10 +2017,13 @@
       </c>
       <c r="F11" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:9">
+        <v>2000</v>
+      </c>
+      <c r="L11" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:12">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2028,9 +2038,12 @@
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="I12" s="3">
         <v>1000</v>
       </c>
-      <c r="I12" s="3">
+      <c r="L12" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2055,7 +2068,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:11">
+    <row r="14" s="3" customFormat="1" spans="1:12">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2073,7 +2086,7 @@
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>9500</v>
+        <v>12000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2086,6 +2099,9 @@
       </c>
       <c r="K14" s="3">
         <v>3000</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2500</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:6">
@@ -2179,7 +2195,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="1" spans="1:6">
+    <row r="19" s="3" customFormat="1" spans="1:12">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2197,7 +2213,10 @@
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="L19" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="1" spans="1:10">
@@ -2314,7 +2333,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:8">
+    <row r="25" s="3" customFormat="1" spans="1:12">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2329,9 +2348,12 @@
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+      <c r="H25" s="3">
         <v>3000</v>
       </c>
-      <c r="H25" s="3">
+      <c r="L25" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -2440,7 +2462,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:6">
+    <row r="31" s="3" customFormat="1" spans="1:12">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2452,7 +2474,10 @@
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="L31" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:8">
@@ -2587,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" s="3" customFormat="1" spans="1:9">
+    <row r="39" s="3" customFormat="1" spans="1:12">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2599,9 +2624,12 @@
       </c>
       <c r="F39" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="I39" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L39" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2755,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:6">
+    <row r="48" s="3" customFormat="1" spans="1:12">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -2773,7 +2801,10 @@
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6000</v>
+      </c>
+      <c r="L48" s="11">
+        <v>6000</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:10">
@@ -2881,7 +2912,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" s="3" customFormat="1" spans="1:6">
+    <row r="54" s="3" customFormat="1" spans="1:12">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2896,7 +2927,10 @@
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="L54" s="3">
+        <v>4000</v>
       </c>
     </row>
     <row r="55" s="3" customFormat="1" spans="1:8">
@@ -2929,7 +2963,10 @@
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="L56" s="3">
+        <v>2000</v>
       </c>
       <c r="AA56" s="3"/>
     </row>
@@ -3038,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" s="3" customFormat="1" spans="1:8">
+    <row r="62" s="3" customFormat="1" spans="1:12">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3050,13 +3087,16 @@
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H62" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="63" s="3" customFormat="1" spans="1:6">
+      <c r="L62" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="63" s="3" customFormat="1" spans="1:12">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3068,7 +3108,10 @@
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="L63" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="64" s="3" customFormat="1" spans="1:6">
@@ -3086,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:9">
+    <row r="65" s="3" customFormat="1" spans="1:12">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3098,7 +3141,7 @@
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -3106,8 +3149,11 @@
       <c r="I65" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="66" s="3" customFormat="1" spans="1:12">
+      <c r="L65" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="66" s="3" customFormat="1" spans="1:8">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3124,7 +3170,6 @@
       <c r="H66" s="3">
         <v>3000</v>
       </c>
-      <c r="L66" s="3"/>
     </row>
     <row r="67" s="3" customFormat="1" spans="1:10">
       <c r="A67" s="3">
@@ -3183,7 +3228,7 @@
       </c>
       <c r="F69" s="10">
         <f t="shared" si="3"/>
-        <v>4100</v>
+        <v>4500</v>
       </c>
       <c r="H69" s="3">
         <v>2800</v>
@@ -3191,9 +3236,12 @@
       <c r="K69" s="3">
         <v>1300</v>
       </c>
+      <c r="L69" s="3">
+        <v>400</v>
+      </c>
       <c r="AE69" s="3"/>
     </row>
-    <row r="70" s="3" customFormat="1" spans="1:9">
+    <row r="70" s="3" customFormat="1" spans="1:12">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -3205,13 +3253,16 @@
       </c>
       <c r="F70" s="10">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="I70" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="71" s="3" customFormat="1" spans="1:8">
+      <c r="L70" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" s="3" customFormat="1" spans="1:12">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3226,9 +3277,12 @@
       </c>
       <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H71" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L71" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3244,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" s="3" customFormat="1" spans="1:6">
+    <row r="73" s="3" customFormat="1" spans="1:12">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -3259,7 +3313,10 @@
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="L73" s="11">
+        <v>3000</v>
       </c>
     </row>
     <row r="74" s="3" customFormat="1" spans="1:6">
@@ -3301,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" s="3" customFormat="1" spans="1:6">
+    <row r="77" s="3" customFormat="1" spans="1:12">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -3313,7 +3370,10 @@
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="L77" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="78" s="3" customFormat="1" spans="1:6">

</xml_diff>

<commit_message>
data updated till 12Jan 8AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>S.No.</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>S K COMMUNICATION(661475194)</t>
+  </si>
+  <si>
+    <t>Abhimanyu</t>
   </si>
   <si>
     <t>SAJNISH KIRANA(661644709)</t>
@@ -579,11 +582,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -611,6 +614,36 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -619,7 +652,76 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -640,98 +742,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -739,19 +749,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -790,7 +793,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +817,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -814,7 +853,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -826,25 +955,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,121 +973,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,6 +984,75 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1012,222 +1084,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1249,7 +1252,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1605,11 +1608,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomRight" activeCell="Q98" sqref="Q98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1746,14 +1749,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>426900</v>
+        <v>480900</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>426900</v>
+        <v>480900</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1797,7 +1800,7 @@
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>54000</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
@@ -1907,10 +1910,13 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="1" spans="1:6">
+    <row r="4" s="3" customFormat="1" spans="1:17">
       <c r="A4" s="3">
         <v>2</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="4">
         <v>9123417146</v>
       </c>
@@ -1918,14 +1924,17 @@
         <v>8</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="1" spans="1:16">
+        <v>1500</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:17">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1936,11 +1945,11 @@
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
@@ -1951,13 +1960,16 @@
       <c r="P5" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:13">
+      <c r="Q5" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:17">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4">
         <v>9102317719</v>
@@ -1966,17 +1978,20 @@
         <v>8</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="H6" s="11">
         <v>3000</v>
       </c>
       <c r="M6" s="3">
         <v>2000</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>3000</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:14">
@@ -1990,7 +2005,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
@@ -2017,7 +2032,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
@@ -2038,7 +2053,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
@@ -2059,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
@@ -2080,16 +2095,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4">
         <v>9973022718</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="1"/>
@@ -2107,10 +2122,10 @@
         <v>7004923653</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
@@ -2137,10 +2152,10 @@
         <v>8340182577</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
@@ -2153,25 +2168,25 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:15">
+    <row r="14" s="3" customFormat="1" spans="1:17">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="4">
         <v>7004740439</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>17500</v>
+        <v>20000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2195,6 +2210,9 @@
         <v>1500</v>
       </c>
       <c r="O14" s="3">
+        <v>2500</v>
+      </c>
+      <c r="Q14" s="11">
         <v>2500</v>
       </c>
     </row>
@@ -2203,14 +2221,14 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
@@ -2225,16 +2243,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4">
         <v>7321004323</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
@@ -2247,31 +2265,34 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="1" spans="1:15">
+    <row r="17" s="3" customFormat="1" spans="1:17">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4">
         <v>9608475282</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>8500</v>
       </c>
       <c r="H17" s="3">
         <v>3000</v>
       </c>
       <c r="O17" s="3">
         <v>3000</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>2500</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:14">
@@ -2282,10 +2303,10 @@
         <v>9661555592</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F18" s="10">
         <f t="shared" si="1"/>
@@ -2303,16 +2324,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="4">
         <v>8340523512</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
@@ -2325,7 +2346,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:10">
+    <row r="20" s="3" customFormat="1" spans="1:17">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2333,17 +2354,20 @@
         <v>8825310472</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J20" s="3">
         <v>2000</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" spans="1:13">
@@ -2351,16 +2375,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4">
         <v>7004478123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F21" s="10">
         <f t="shared" si="1"/>
@@ -2373,7 +2397,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:11">
+    <row r="22" s="3" customFormat="1" spans="1:17">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2381,19 +2405,22 @@
         <v>7667895364</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="H22" s="3">
         <v>1000</v>
       </c>
       <c r="K22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q22" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2402,16 +2429,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4">
         <v>7006041121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
@@ -2426,16 +2453,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="4">
         <v>8709658240</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="1"/>
@@ -2451,7 +2478,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:14">
+    <row r="25" s="3" customFormat="1" spans="1:17">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2459,14 +2486,14 @@
         <v>8709612020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
@@ -2475,6 +2502,9 @@
         <v>3000</v>
       </c>
       <c r="N25" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Q25" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2486,10 +2516,10 @@
         <v>9973040600</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F26" s="10">
         <f t="shared" si="1"/>
@@ -2516,10 +2546,10 @@
         <v>9973345687</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" si="1"/>
@@ -2537,10 +2567,10 @@
         <v>9631391206</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="1"/>
@@ -2558,13 +2588,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F29" s="10">
         <f t="shared" si="1"/>
@@ -2579,13 +2609,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F30" s="10">
         <f t="shared" si="1"/>
@@ -2604,19 +2634,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:14">
+    <row r="31" s="3" customFormat="1" spans="1:17">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -2624,29 +2654,35 @@
       <c r="N31" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="32" s="3" customFormat="1" spans="1:13">
+      <c r="Q31" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" s="3" customFormat="1" spans="1:17">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F32" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H32" s="3">
         <v>1000</v>
       </c>
       <c r="M32" s="11">
         <v>1000</v>
+      </c>
+      <c r="Q32" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" spans="1:13">
@@ -2654,10 +2690,10 @@
         <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" si="1"/>
@@ -2678,10 +2714,10 @@
         <v>7654800030</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F34" s="10">
         <f t="shared" si="1"/>
@@ -2697,19 +2733,19 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:15">
+    <row r="35" s="3" customFormat="1" spans="1:17">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F35" s="10">
         <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="K35" s="11">
         <v>3000</v>
@@ -2718,6 +2754,9 @@
         <v>3000</v>
       </c>
       <c r="O35" s="11">
+        <v>3000</v>
+      </c>
+      <c r="Q35" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2726,10 +2765,10 @@
         <v>34</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="2"/>
@@ -2744,13 +2783,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" si="2"/>
@@ -2771,10 +2810,10 @@
         <v>36</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
@@ -2786,10 +2825,10 @@
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F39" s="10">
         <f t="shared" si="2"/>
@@ -2810,10 +2849,10 @@
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F40" s="10">
         <f t="shared" si="2"/>
@@ -2823,7 +2862,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:14">
+    <row r="41" s="3" customFormat="1" spans="1:17">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2831,14 +2870,14 @@
         <v>8210095108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>18000</v>
       </c>
       <c r="H41" s="3">
         <v>6000</v>
@@ -2848,6 +2887,9 @@
       </c>
       <c r="N41" s="3">
         <v>3000</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>6000</v>
       </c>
     </row>
     <row r="42" s="3" customFormat="1" spans="1:8">
@@ -2855,10 +2897,10 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F42" s="10">
         <f t="shared" si="2"/>
@@ -2873,29 +2915,29 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:13">
+    <row r="44" s="3" customFormat="1" spans="1:17">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H44" s="3">
         <v>3000</v>
@@ -2904,6 +2946,9 @@
         <v>3000</v>
       </c>
       <c r="M44" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Q44" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2912,10 +2957,10 @@
         <v>43</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F45" s="10">
         <f t="shared" si="2"/>
@@ -2931,24 +2976,27 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:13">
+    <row r="46" s="3" customFormat="1" spans="1:17">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F46" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="I46" s="3">
         <v>3000</v>
       </c>
       <c r="M46" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Q46" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2957,13 +3005,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F47" s="10">
         <f t="shared" si="2"/>
@@ -2973,28 +3021,31 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:12">
+    <row r="48" s="3" customFormat="1" spans="1:17">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="L48" s="11">
         <v>6000</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:13">
@@ -3002,16 +3053,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F49" s="10">
         <f t="shared" si="2"/>
@@ -3029,13 +3080,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F50" s="10">
         <f t="shared" si="2"/>
@@ -3048,37 +3099,40 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" s="3" customFormat="1" spans="1:6">
+    <row r="51" s="3" customFormat="1" spans="1:17">
       <c r="A51" s="3">
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F51" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" s="3" customFormat="1" spans="1:15">
+        <v>1000</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" s="3" customFormat="1" spans="1:17">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>10000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -3092,8 +3146,11 @@
       <c r="O52" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="53" s="3" customFormat="1" spans="1:15">
+      <c r="Q52" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="1" spans="1:17">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3101,14 +3158,14 @@
         <v>6202424016</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F53" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="J53" s="11">
         <v>2000</v>
@@ -3117,6 +3174,9 @@
         <v>1000</v>
       </c>
       <c r="O53" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q53" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3128,10 +3188,10 @@
         <v>7004211364</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
@@ -3146,13 +3206,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
@@ -3170,10 +3230,10 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
@@ -3189,16 +3249,16 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C57" s="3">
         <v>9504958065</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F57" s="10">
         <f t="shared" si="2"/>
@@ -3219,13 +3279,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F58" s="10">
         <f t="shared" si="2"/>
@@ -3240,13 +3300,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F59" s="10">
         <f t="shared" si="2"/>
@@ -3270,10 +3330,10 @@
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F60" s="10">
         <f t="shared" si="2"/>
@@ -3288,10 +3348,10 @@
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F61" s="10">
         <f t="shared" si="2"/>
@@ -3301,24 +3361,27 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="62" s="3" customFormat="1" spans="1:12">
+    <row r="62" s="3" customFormat="1" spans="1:17">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H62" s="3">
         <v>2000</v>
       </c>
       <c r="L62" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Q62" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3327,10 +3390,10 @@
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
@@ -3345,10 +3408,10 @@
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F64" s="10">
         <f t="shared" si="2"/>
@@ -3358,19 +3421,19 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:12">
+    <row r="65" s="3" customFormat="1" spans="1:17">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -3380,6 +3443,9 @@
       </c>
       <c r="L65" s="3">
         <v>5000</v>
+      </c>
+      <c r="Q65" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="66" s="3" customFormat="1" spans="1:14">
@@ -3387,10 +3453,10 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
@@ -3408,16 +3474,16 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C67" s="3">
         <v>8825370430</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F67" s="10">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
@@ -3435,10 +3501,10 @@
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F68" s="10">
         <f t="shared" si="3"/>
@@ -3456,14 +3522,14 @@
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F69" s="10">
         <f t="shared" si="3"/>
-        <v>5100</v>
+        <v>5600</v>
       </c>
       <c r="H69" s="3">
         <v>2800</v>
@@ -3476,6 +3542,9 @@
       </c>
       <c r="O69" s="3">
         <v>600</v>
+      </c>
+      <c r="Q69" s="3">
+        <v>500</v>
       </c>
       <c r="AE69" s="3"/>
     </row>
@@ -3484,10 +3553,10 @@
         <v>68</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F70" s="10">
         <f t="shared" si="3"/>
@@ -3503,22 +3572,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="71" s="3" customFormat="1" spans="1:14">
+    <row r="71" s="3" customFormat="1" spans="1:17">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H71" s="3">
         <v>2000</v>
@@ -3527,6 +3596,9 @@
         <v>2000</v>
       </c>
       <c r="N71" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Q71" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3535,7 +3607,7 @@
         <v>70</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F72" s="10">
         <f t="shared" si="3"/>
@@ -3547,13 +3619,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
@@ -3568,7 +3640,7 @@
         <v>72</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F74" s="10">
         <f t="shared" si="3"/>
@@ -3580,10 +3652,10 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F75" s="10">
         <f t="shared" si="3"/>
@@ -3598,7 +3670,7 @@
         <v>74</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F76" s="10">
         <f t="shared" si="3"/>
@@ -3610,10 +3682,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
@@ -3628,7 +3700,7 @@
         <v>76</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F78" s="10">
         <f t="shared" si="3"/>
@@ -3643,7 +3715,7 @@
         <v>77</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F79" s="10">
         <f t="shared" si="3"/>
@@ -3655,7 +3727,7 @@
         <v>78</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F80" s="10">
         <f t="shared" si="3"/>
@@ -3667,7 +3739,7 @@
         <v>79</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F81" s="10">
         <f t="shared" si="3"/>
@@ -3682,10 +3754,10 @@
         <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
@@ -3706,7 +3778,7 @@
         <v>81</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F83" s="10">
         <f t="shared" si="3"/>
@@ -3718,7 +3790,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F84" s="10">
         <f t="shared" si="3"/>
@@ -3730,13 +3802,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F85" s="10">
         <f t="shared" si="3"/>
@@ -3748,7 +3820,7 @@
         <v>84</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F86" s="10">
         <f t="shared" si="3"/>
@@ -3760,7 +3832,7 @@
         <v>85</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F87" s="10">
         <f t="shared" si="3"/>
@@ -3772,7 +3844,7 @@
         <v>86</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F88" s="10">
         <f t="shared" si="3"/>
@@ -3784,7 +3856,7 @@
         <v>87</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F89" s="10">
         <f t="shared" si="3"/>
@@ -3796,7 +3868,7 @@
         <v>88</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
@@ -3808,7 +3880,7 @@
         <v>89</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
@@ -3820,7 +3892,7 @@
         <v>90</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F92" s="10">
         <f t="shared" si="3"/>
@@ -3832,7 +3904,7 @@
         <v>91</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F93" s="10">
         <f t="shared" si="3"/>
@@ -3844,7 +3916,7 @@
         <v>92</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F94" s="10">
         <f t="shared" si="3"/>
@@ -3856,13 +3928,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F95" s="10">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
data updated till 16Dec 11AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -161,6 +161,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="U69" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+600-Cash
+1500-Digital</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AE69" authorId="0">
       <text>
         <r>
@@ -189,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
   <si>
     <t>S.No.</t>
   </si>
@@ -518,6 +541,9 @@
     <t>RAJESH TELECOM &amp; KIRANA DUKAN(661063895)</t>
   </si>
   <si>
+    <t>Brajesh Kr.</t>
+  </si>
+  <si>
     <t>BELSAR</t>
   </si>
   <si>
@@ -569,7 +595,13 @@
     <t>SONU PHONE GHAR(660815245)</t>
   </si>
   <si>
+    <t>Binod Kr. Vishwaka</t>
+  </si>
+  <si>
     <t>SANGAM GENERAL STORE(661644708)</t>
+  </si>
+  <si>
+    <t>Rupsagar</t>
   </si>
   <si>
     <t>sugam phone bathe(661711006)</t>
@@ -631,10 +663,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -654,16 +686,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,14 +701,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -691,9 +708,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -709,7 +734,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -724,30 +749,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -755,6 +786,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -769,6 +808,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -777,22 +824,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -842,13 +874,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,7 +952,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +976,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,25 +988,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -914,115 +1048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,11 +1068,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1060,32 +1113,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1093,8 +1127,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1125,11 +1159,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1138,15 +1170,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1156,130 +1188,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1657,11 +1689,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="K34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1798,14 +1830,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>534400</v>
+        <v>670500</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>534400</v>
+        <v>670500</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1857,15 +1889,15 @@
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>41000</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>93100</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
@@ -2016,7 +2048,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" spans="1:18">
+    <row r="6" s="3" customFormat="1" spans="1:21">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2034,7 +2066,7 @@
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="H6" s="11">
         <v>3000</v>
@@ -2047,6 +2079,9 @@
       </c>
       <c r="R6" s="11">
         <v>2000</v>
+      </c>
+      <c r="U6" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:18">
@@ -2100,7 +2135,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:11">
+    <row r="9" s="3" customFormat="1" spans="1:21">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2115,13 +2150,16 @@
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K9" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="10" s="3" customFormat="1" spans="1:16">
+      <c r="U9" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="1" spans="1:21">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2136,7 +2174,7 @@
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K10" s="3">
         <v>5000</v>
@@ -2146,6 +2184,9 @@
       </c>
       <c r="P10" s="3">
         <v>1000</v>
+      </c>
+      <c r="U10" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:18">
@@ -2175,7 +2216,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="1" spans="1:18">
+    <row r="12" s="3" customFormat="1" spans="1:21">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2190,7 +2231,7 @@
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
-        <v>3500</v>
+        <v>5000</v>
       </c>
       <c r="I12" s="3">
         <v>1000</v>
@@ -2207,8 +2248,14 @@
       <c r="R12" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:15">
+      <c r="S12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="U12" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:21">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2223,7 +2270,7 @@
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="I13" s="3">
         <v>5000</v>
@@ -2231,8 +2278,11 @@
       <c r="O13" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:18">
+      <c r="U13" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:21">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2250,7 +2300,7 @@
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>22500</v>
+        <v>30000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2282,8 +2332,14 @@
       <c r="R14" s="3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:13">
+      <c r="S14" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U14" s="3">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:21">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2299,9 +2355,12 @@
       </c>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="M15" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U15" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2332,7 +2391,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="1" spans="1:17">
+    <row r="17" s="3" customFormat="1" spans="1:19">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2350,7 +2409,7 @@
       </c>
       <c r="F17" s="10">
         <f t="shared" si="1"/>
-        <v>8500</v>
+        <v>12000</v>
       </c>
       <c r="H17" s="3">
         <v>3000</v>
@@ -2360,6 +2419,9 @@
       </c>
       <c r="Q17" s="3">
         <v>2500</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3500</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:14">
@@ -2467,7 +2529,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:17">
+    <row r="22" s="3" customFormat="1" spans="1:21">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2482,7 +2544,7 @@
       </c>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="H22" s="3">
         <v>1000</v>
@@ -2493,8 +2555,11 @@
       <c r="Q22" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" s="3" customFormat="1" spans="1:18">
+      <c r="U22" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:21">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2512,7 +2577,7 @@
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="P23" s="11">
         <v>3000</v>
@@ -2520,8 +2585,11 @@
       <c r="R23" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="24" s="3" customFormat="1" spans="1:15">
+      <c r="U23" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="1" spans="1:20">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2539,7 +2607,7 @@
       </c>
       <c r="F24" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H24" s="11">
         <v>5000</v>
@@ -2548,6 +2616,9 @@
         <v>5000</v>
       </c>
       <c r="O24" s="11">
+        <v>5000</v>
+      </c>
+      <c r="T24" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -2584,7 +2655,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="26" s="3" customFormat="1" spans="1:15">
+    <row r="26" s="3" customFormat="1" spans="1:21">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2599,7 +2670,7 @@
       </c>
       <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="H26" s="3">
         <v>1000</v>
@@ -2613,8 +2684,11 @@
       <c r="O26" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" s="3" customFormat="1" spans="1:8">
+      <c r="U26" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" s="3" customFormat="1" spans="1:21">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2629,9 +2703,12 @@
       </c>
       <c r="F27" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H27" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U27" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2683,7 +2760,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" s="3" customFormat="1" spans="1:16">
+    <row r="30" s="3" customFormat="1" spans="1:21">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2698,7 +2775,7 @@
       </c>
       <c r="F30" s="10">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>35000</v>
       </c>
       <c r="H30" s="3">
         <v>10000</v>
@@ -2712,8 +2789,14 @@
       <c r="P30" s="11">
         <v>5000</v>
       </c>
-    </row>
-    <row r="31" s="3" customFormat="1" spans="1:18">
+      <c r="S30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U30" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" s="3" customFormat="1" spans="1:21">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2725,7 +2808,7 @@
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>3500</v>
+        <v>5000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -2738,6 +2821,12 @@
       </c>
       <c r="R31" s="3">
         <v>500</v>
+      </c>
+      <c r="S31" s="3">
+        <v>500</v>
+      </c>
+      <c r="U31" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:17">
@@ -2767,7 +2856,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="33" s="3" customFormat="1" spans="1:13">
+    <row r="33" s="3" customFormat="1" spans="1:21">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2779,7 +2868,7 @@
       </c>
       <c r="F33" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J33" s="3">
         <v>1000</v>
@@ -2787,8 +2876,11 @@
       <c r="M33" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="34" s="3" customFormat="1" spans="1:19">
+      <c r="U33" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" s="3" customFormat="1" spans="1:21">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2803,7 +2895,7 @@
       </c>
       <c r="F34" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="H34" s="3">
         <v>1000</v>
@@ -2817,8 +2909,11 @@
       <c r="S34" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="35" s="3" customFormat="1" spans="1:17">
+      <c r="U34" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" s="3" customFormat="1" spans="1:20">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2830,7 +2925,7 @@
       </c>
       <c r="F35" s="10">
         <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="K35" s="11">
         <v>3000</v>
@@ -2844,8 +2939,11 @@
       <c r="Q35" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="36" s="3" customFormat="1" spans="1:15">
+      <c r="T35" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="36" s="3" customFormat="1" spans="1:19">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2857,13 +2955,16 @@
       </c>
       <c r="F36" s="10">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="O36" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="37" s="3" customFormat="1" spans="1:16">
+      <c r="S36" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" s="3" customFormat="1" spans="1:21">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2878,7 +2979,7 @@
       </c>
       <c r="F37" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H37" s="11">
         <v>3000</v>
@@ -2889,8 +2990,11 @@
       <c r="P37" s="11">
         <v>3000</v>
       </c>
-    </row>
-    <row r="38" s="3" customFormat="1" spans="1:6">
+      <c r="U37" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="38" s="3" customFormat="1" spans="1:21">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -2902,10 +3006,13 @@
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" s="3" customFormat="1" spans="1:15">
+        <v>2000</v>
+      </c>
+      <c r="U38" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" s="3" customFormat="1" spans="1:21">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2917,7 +3024,7 @@
       </c>
       <c r="F39" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="I39" s="3">
         <v>2000</v>
@@ -2926,6 +3033,9 @@
         <v>2000</v>
       </c>
       <c r="O39" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U39" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2950,7 +3060,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:19">
+    <row r="41" s="3" customFormat="1" spans="1:21">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2965,7 +3075,7 @@
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="H41" s="3">
         <v>6000</v>
@@ -2980,6 +3090,9 @@
         <v>3000</v>
       </c>
       <c r="S41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U41" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3016,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:17">
+    <row r="44" s="3" customFormat="1" spans="1:19">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3028,7 +3141,7 @@
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H44" s="3">
         <v>3000</v>
@@ -3040,6 +3153,9 @@
         <v>3000</v>
       </c>
       <c r="Q44" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S44" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3112,7 +3228,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:17">
+    <row r="48" s="3" customFormat="1" spans="1:19">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3130,13 +3246,16 @@
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="L48" s="11">
         <v>6000</v>
       </c>
       <c r="Q48" s="3">
         <v>3000</v>
+      </c>
+      <c r="S48" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:18">
@@ -3214,7 +3333,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:17">
+    <row r="52" s="3" customFormat="1" spans="1:19">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3229,7 +3348,7 @@
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -3244,6 +3363,9 @@
         <v>1000</v>
       </c>
       <c r="Q52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="S52" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3277,7 +3399,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="54" s="3" customFormat="1" spans="1:12">
+    <row r="54" s="3" customFormat="1" spans="1:21">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3292,13 +3414,16 @@
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="L54" s="3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="55" s="3" customFormat="1" spans="1:13">
+      <c r="U54" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="55" s="3" customFormat="1" spans="1:21">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -3313,12 +3438,18 @@
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
       </c>
       <c r="M55" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S55" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U55" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3334,14 +3465,17 @@
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L56" s="3">
         <v>2000</v>
       </c>
+      <c r="U56" s="3">
+        <v>2000</v>
+      </c>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" s="3" customFormat="1" spans="1:14">
+    <row r="57" s="3" customFormat="1" spans="1:21">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -3359,7 +3493,7 @@
       </c>
       <c r="F57" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H57" s="11">
         <v>5000</v>
@@ -3370,8 +3504,11 @@
       <c r="N57" s="11">
         <v>5000</v>
       </c>
-    </row>
-    <row r="58" s="3" customFormat="1" spans="1:9">
+      <c r="U57" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="58" s="3" customFormat="1" spans="1:21">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -3386,13 +3523,16 @@
       </c>
       <c r="F58" s="10">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="I58" s="11">
         <v>5000</v>
       </c>
-    </row>
-    <row r="59" s="3" customFormat="1" spans="1:16">
+      <c r="U58" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="59" s="3" customFormat="1" spans="1:19">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -3407,7 +3547,7 @@
       </c>
       <c r="F59" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>11000</v>
       </c>
       <c r="G59" s="11">
         <v>2000</v>
@@ -3419,6 +3559,9 @@
         <v>2000</v>
       </c>
       <c r="P59" s="11">
+        <v>2000</v>
+      </c>
+      <c r="S59" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3443,7 +3586,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="61" s="3" customFormat="1" spans="1:14">
+    <row r="61" s="3" customFormat="1" spans="1:21">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3455,13 +3598,16 @@
       </c>
       <c r="F61" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="N61" s="3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="62" s="3" customFormat="1" spans="1:17">
+      <c r="U61" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="62" s="3" customFormat="1" spans="1:21">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3473,7 +3619,7 @@
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H62" s="3">
         <v>2000</v>
@@ -3484,8 +3630,11 @@
       <c r="Q62" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="63" s="3" customFormat="1" spans="1:12">
+      <c r="U62" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="63" s="3" customFormat="1" spans="1:21">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3497,9 +3646,12 @@
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L63" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U63" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3521,7 +3673,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:17">
+    <row r="65" s="3" customFormat="1" spans="1:21">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3533,7 +3685,7 @@
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -3547,8 +3699,11 @@
       <c r="Q65" s="3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="66" s="3" customFormat="1" spans="1:18">
+      <c r="U65" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="66" s="3" customFormat="1" spans="1:21">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3560,7 +3715,7 @@
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H66" s="3">
         <v>3000</v>
@@ -3569,6 +3724,9 @@
         <v>6000</v>
       </c>
       <c r="R66" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U66" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -3624,18 +3782,21 @@
       <c r="A69" s="3">
         <v>67</v>
       </c>
+      <c r="B69" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="C69" s="3">
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F69" s="10">
         <f t="shared" si="3"/>
-        <v>5600</v>
+        <v>7700</v>
       </c>
       <c r="H69" s="3">
         <v>2800</v>
@@ -3652,24 +3813,27 @@
       <c r="Q69" s="3">
         <v>500</v>
       </c>
+      <c r="U69" s="11">
+        <v>2100</v>
+      </c>
       <c r="AE69" s="3"/>
     </row>
-    <row r="70" s="3" customFormat="1" spans="1:18">
+    <row r="70" s="3" customFormat="1" spans="1:21">
       <c r="A70" s="3">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F70" s="10">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="I70" s="3">
         <v>3000</v>
@@ -3683,23 +3847,26 @@
       <c r="R70" s="11">
         <v>3000</v>
       </c>
-    </row>
-    <row r="71" s="3" customFormat="1" spans="1:17">
+      <c r="U70" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" s="3" customFormat="1" spans="1:21">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="H71" s="3">
         <v>2000</v>
@@ -3711,6 +3878,12 @@
         <v>2000</v>
       </c>
       <c r="Q71" s="11">
+        <v>2000</v>
+      </c>
+      <c r="S71" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U71" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3719,7 +3892,7 @@
         <v>70</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F72" s="10">
         <f t="shared" si="3"/>
@@ -3731,13 +3904,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
@@ -3752,28 +3925,31 @@
         <v>72</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F74" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" s="3" customFormat="1" spans="1:13">
+    <row r="75" s="3" customFormat="1" spans="1:21">
       <c r="A75" s="3">
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F75" s="10">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="M75" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U75" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3782,7 +3958,7 @@
         <v>74</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F76" s="10">
         <f t="shared" si="3"/>
@@ -3797,7 +3973,7 @@
         <v>34</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
@@ -3811,8 +3987,11 @@
       <c r="A78" s="3">
         <v>76</v>
       </c>
+      <c r="D78" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="E78" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F78" s="10">
         <f t="shared" si="3"/>
@@ -3827,31 +4006,46 @@
         <v>77</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F79" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" s="3" customFormat="1" spans="1:6">
+    <row r="80" s="3" customFormat="1" spans="1:21">
       <c r="A80" s="3">
         <v>78</v>
       </c>
+      <c r="B80" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="E80" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F80" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="S80" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U80" s="11">
+        <v>1000</v>
       </c>
     </row>
     <row r="81" s="3" customFormat="1" spans="1:11">
       <c r="A81" s="3">
         <v>79</v>
       </c>
+      <c r="D81" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="E81" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F81" s="10">
         <f t="shared" si="3"/>
@@ -3861,19 +4055,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="82" s="3" customFormat="1" spans="1:16">
+    <row r="82" s="3" customFormat="1" spans="1:19">
       <c r="A82" s="3">
         <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H82" s="11">
         <v>5000</v>
@@ -3882,6 +4076,9 @@
         <v>5000</v>
       </c>
       <c r="P82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S82" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -3890,7 +4087,7 @@
         <v>81</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F83" s="10">
         <f t="shared" si="3"/>
@@ -3902,7 +4099,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F84" s="10">
         <f t="shared" si="3"/>
@@ -3914,13 +4111,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F85" s="10">
         <f t="shared" si="3"/>
@@ -3932,7 +4129,7 @@
         <v>84</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F86" s="10">
         <f t="shared" si="3"/>
@@ -3944,7 +4141,7 @@
         <v>85</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F87" s="10">
         <f t="shared" si="3"/>
@@ -3956,7 +4153,7 @@
         <v>86</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F88" s="10">
         <f t="shared" si="3"/>
@@ -3968,7 +4165,7 @@
         <v>87</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F89" s="10">
         <f t="shared" si="3"/>
@@ -3980,7 +4177,7 @@
         <v>88</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
@@ -3992,7 +4189,7 @@
         <v>89</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
@@ -4004,7 +4201,7 @@
         <v>90</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F92" s="10">
         <f t="shared" si="3"/>
@@ -4016,7 +4213,7 @@
         <v>91</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F93" s="10">
         <f t="shared" si="3"/>
@@ -4028,7 +4225,7 @@
         <v>92</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F94" s="10">
         <f t="shared" si="3"/>
@@ -4040,13 +4237,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F95" s="10">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
data updated till 17Jan 2021 8AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="154">
   <si>
     <t>S.No.</t>
   </si>
@@ -247,6 +247,9 @@
     <t>Abhimanyu</t>
   </si>
   <si>
+    <t>9123417146/7979995728</t>
+  </si>
+  <si>
     <t>SAJNISH KIRANA(661644709)</t>
   </si>
   <si>
@@ -400,6 +403,9 @@
     <t>MS OM COMPUTER(661542289)</t>
   </si>
   <si>
+    <t>8709954402/6207783075</t>
+  </si>
+  <si>
     <t>SANTU KIRANA STORE(661752211)</t>
   </si>
   <si>
@@ -493,6 +499,9 @@
     <t>Amresh Kr.</t>
   </si>
   <si>
+    <t>9931812966/9572985032</t>
+  </si>
+  <si>
     <t>MAA VINDHYAVASINI MOBILE CENTE(660064218)</t>
   </si>
   <si>
@@ -568,6 +577,9 @@
     <t>INDRJEET KUMAR</t>
   </si>
   <si>
+    <t>8789783884/7061621223</t>
+  </si>
+  <si>
     <t>Dhewai</t>
   </si>
   <si>
@@ -607,6 +619,9 @@
     <t>sugam phone bathe(661711006)</t>
   </si>
   <si>
+    <t>Khatri sudhir sahani</t>
+  </si>
+  <si>
     <t>Arwal</t>
   </si>
   <si>
@@ -620,6 +635,9 @@
   </si>
   <si>
     <t>Sabbir Ahmad</t>
+  </si>
+  <si>
+    <t>9122226169/6200715559</t>
   </si>
   <si>
     <t>KRISHNA KIRANA STORE(661613674)</t>
@@ -663,11 +681,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -686,9 +704,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,8 +733,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -710,15 +743,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,14 +766,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -749,29 +774,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -785,14 +788,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -800,8 +795,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -817,14 +813,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -874,7 +892,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,13 +922,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -904,37 +1006,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,7 +1018,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,37 +1036,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,61 +1060,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,32 +1086,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1115,17 +1138,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1134,16 +1146,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,11 +1169,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1170,15 +1188,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1188,138 +1206,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1333,7 +1351,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1354,6 +1375,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1689,11 +1718,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="M38" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U23" sqref="U23"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1712,132 +1741,132 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:37">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="6">
         <v>44197</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="6">
         <v>44198</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="6">
         <v>44199</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="6">
         <v>44200</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="6">
         <v>44201</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="6">
         <v>44202</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="6">
         <v>44203</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="6">
         <v>44204</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="6">
         <v>44205</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="6">
         <v>44206</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="6">
         <v>44207</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="6">
         <v>44208</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="6">
         <v>44209</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="6">
         <v>44210</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="6">
         <v>44211</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="6">
         <v>44212</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="6">
         <v>44213</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="6">
         <v>44214</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="6">
         <v>44215</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="6">
         <v>44216</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="6">
         <v>44217</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="6">
         <v>44218</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AC1" s="6">
         <v>44219</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AD1" s="6">
         <v>44220</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AE1" s="6">
         <v>44221</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AF1" s="6">
         <v>44222</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AG1" s="6">
         <v>44223</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AH1" s="6">
         <v>44224</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AI1" s="6">
         <v>44225</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AJ1" s="6">
         <v>44226</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AK1" s="6">
         <v>44227</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:37">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8">
         <f>SUM(F3:F120)</f>
-        <v>670500</v>
-      </c>
-      <c r="E2" s="8" t="s">
+        <v>713000</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <f>SUM(G2:AK2)</f>
-        <v>670500</v>
+        <v>713000</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1901,7 +1930,7 @@
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42500</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
@@ -1977,17 +2006,17 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="11">
         <f t="shared" ref="F3:F34" si="1">SUM(G3:AK3)</f>
         <v>6000</v>
       </c>
-      <c r="H3" s="11">
-        <v>3000</v>
-      </c>
-      <c r="M3" s="11">
+      <c r="H3" s="12">
+        <v>3000</v>
+      </c>
+      <c r="M3" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -1998,20 +2027,20 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <v>9123417146</v>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="E4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="11">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="12">
         <v>1500</v>
       </c>
     </row>
@@ -2025,10 +2054,10 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="11">
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
@@ -2053,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4">
         <v>9102317719</v>
@@ -2061,23 +2090,23 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="11">
         <f t="shared" si="1"/>
         <v>13000</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="12">
         <v>3000</v>
       </c>
       <c r="M6" s="3">
         <v>2000</v>
       </c>
-      <c r="Q6" s="11">
-        <v>3000</v>
-      </c>
-      <c r="R6" s="11">
+      <c r="Q6" s="12">
+        <v>3000</v>
+      </c>
+      <c r="R6" s="12">
         <v>2000</v>
       </c>
       <c r="U6" s="3">
@@ -2094,23 +2123,23 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11">
         <f t="shared" si="1"/>
         <v>25000</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="12">
         <v>4000</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="12">
         <v>7000</v>
       </c>
       <c r="N7" s="3">
         <v>4000</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="12">
         <v>10000</v>
       </c>
     </row>
@@ -2124,10 +2153,10 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="11">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
@@ -2145,10 +2174,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2169,10 +2198,10 @@
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="11">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
@@ -2194,25 +2223,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <v>9973022718</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="10">
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="11">
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
-      <c r="L11" s="11">
-        <v>2000</v>
-      </c>
-      <c r="R11" s="11">
+      <c r="L11" s="12">
+        <v>2000</v>
+      </c>
+      <c r="R11" s="12">
         <v>4000</v>
       </c>
     </row>
@@ -2224,12 +2253,12 @@
         <v>7004923653</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="10">
+        <v>21</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
@@ -2263,12 +2292,12 @@
         <v>8340182577</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="10">
+        <v>21</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
@@ -2282,25 +2311,25 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:21">
+    <row r="14" s="3" customFormat="1" spans="1:22">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4">
         <v>7004740439</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="10">
+        <v>21</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="11">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>31000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2308,7 +2337,7 @@
       <c r="I14" s="3">
         <v>2500</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="12">
         <v>1500</v>
       </c>
       <c r="K14" s="3">
@@ -2317,7 +2346,7 @@
       <c r="L14" s="3">
         <v>2500</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="12">
         <v>1500</v>
       </c>
       <c r="N14" s="3">
@@ -2326,7 +2355,7 @@
       <c r="O14" s="3">
         <v>2500</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="Q14" s="12">
         <v>2500</v>
       </c>
       <c r="R14" s="3">
@@ -2337,6 +2366,9 @@
       </c>
       <c r="U14" s="3">
         <v>5500</v>
+      </c>
+      <c r="V14" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:21">
@@ -2344,16 +2376,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="10">
+        <v>21</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2369,18 +2401,18 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4">
         <v>7321004323</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="10">
+        <v>21</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="11">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
@@ -2396,18 +2428,18 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4">
         <v>9608475282</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="10">
+        <v>21</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="11">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
@@ -2424,7 +2456,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="1" spans="1:14">
+    <row r="18" s="3" customFormat="1" spans="1:22">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2432,19 +2464,22 @@
         <v>9661555592</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="10">
+      <c r="E18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="11">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="J18" s="3">
         <v>5000</v>
       </c>
       <c r="N18" s="3">
+        <v>5000</v>
+      </c>
+      <c r="V18" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -2453,25 +2488,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4">
         <v>8340523512</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="10">
+        <v>33</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="L19" s="11">
-        <v>2000</v>
-      </c>
-      <c r="P19" s="11">
+      <c r="L19" s="12">
+        <v>2000</v>
+      </c>
+      <c r="P19" s="12">
         <v>2000</v>
       </c>
     </row>
@@ -2483,12 +2518,12 @@
         <v>8825310472</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="10">
+        <v>33</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="11">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
@@ -2504,32 +2539,32 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="4">
         <v>7004478123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="10">
+        <v>33</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="11">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="H21" s="11">
-        <v>5000</v>
-      </c>
-      <c r="M21" s="11">
-        <v>5000</v>
-      </c>
-      <c r="R21" s="11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="1" spans="1:21">
+      <c r="H21" s="12">
+        <v>5000</v>
+      </c>
+      <c r="M21" s="12">
+        <v>5000</v>
+      </c>
+      <c r="R21" s="12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:22">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2537,14 +2572,14 @@
         <v>7667895364</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="10">
+        <v>33</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="11">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="H22" s="3">
         <v>1000</v>
@@ -2556,6 +2591,9 @@
         <v>1000</v>
       </c>
       <c r="U22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V22" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2564,22 +2602,22 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="4">
         <v>7006041121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="10">
+        <v>33</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="11">
         <f t="shared" si="1"/>
         <v>9000</v>
       </c>
-      <c r="P23" s="11">
+      <c r="P23" s="12">
         <v>3000</v>
       </c>
       <c r="R23" s="3">
@@ -2594,35 +2632,35 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4">
         <v>8709658240</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="10">
+        <v>33</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="11">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="H24" s="11">
-        <v>5000</v>
-      </c>
-      <c r="J24" s="11">
-        <v>5000</v>
-      </c>
-      <c r="O24" s="11">
-        <v>5000</v>
-      </c>
-      <c r="T24" s="11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="25" s="3" customFormat="1" spans="1:18">
+      <c r="H24" s="12">
+        <v>5000</v>
+      </c>
+      <c r="J24" s="12">
+        <v>5000</v>
+      </c>
+      <c r="O24" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T24" s="12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="1" spans="1:22">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2630,19 +2668,19 @@
         <v>8709612020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="10">
+        <v>33</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="11">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>17500</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="12">
         <v>3000</v>
       </c>
       <c r="N25" s="3">
@@ -2653,6 +2691,9 @@
       </c>
       <c r="R25" s="3">
         <v>3000</v>
+      </c>
+      <c r="V25" s="3">
+        <v>2500</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" spans="1:21">
@@ -2663,12 +2704,12 @@
         <v>9973040600</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="10">
+        <v>33</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="11">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
@@ -2696,12 +2737,12 @@
         <v>9973345687</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="10">
+        <v>33</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2720,12 +2761,12 @@
         <v>9631391206</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="10">
+        <v>33</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2741,22 +2782,22 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="10">
+        <v>33</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="11">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="M29" s="11">
-        <v>5000</v>
-      </c>
-      <c r="R29" s="11">
+      <c r="M29" s="12">
+        <v>5000</v>
+      </c>
+      <c r="R29" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -2765,34 +2806,34 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="10">
+        <v>33</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="11">
         <f t="shared" si="1"/>
         <v>35000</v>
       </c>
       <c r="H30" s="3">
         <v>10000</v>
       </c>
-      <c r="K30" s="11">
-        <v>5000</v>
-      </c>
-      <c r="M30" s="11">
-        <v>5000</v>
-      </c>
-      <c r="P30" s="11">
-        <v>5000</v>
-      </c>
-      <c r="S30" s="11">
-        <v>5000</v>
-      </c>
-      <c r="U30" s="11">
+      <c r="K30" s="12">
+        <v>5000</v>
+      </c>
+      <c r="M30" s="12">
+        <v>5000</v>
+      </c>
+      <c r="P30" s="12">
+        <v>5000</v>
+      </c>
+      <c r="S30" s="12">
+        <v>5000</v>
+      </c>
+      <c r="U30" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -2801,12 +2842,12 @@
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="10">
+        <v>33</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="11">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
@@ -2829,47 +2870,50 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" s="3" customFormat="1" spans="1:17">
+    <row r="32" s="3" customFormat="1" spans="1:22">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="10">
+      <c r="E32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1000</v>
+      </c>
+      <c r="M32" s="12">
+        <v>1000</v>
+      </c>
+      <c r="Q32" s="12">
+        <v>2000</v>
+      </c>
+      <c r="V32" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" s="3" customFormat="1" spans="1:22">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="11">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="H32" s="3">
-        <v>1000</v>
-      </c>
-      <c r="M32" s="11">
-        <v>1000</v>
-      </c>
-      <c r="Q32" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="33" s="3" customFormat="1" spans="1:21">
-      <c r="A33" s="3">
-        <v>31</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="10">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
       <c r="J33" s="3">
         <v>1000</v>
       </c>
@@ -2877,6 +2921,9 @@
         <v>1000</v>
       </c>
       <c r="U33" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V33" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2888,12 +2935,12 @@
         <v>7654800030</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="10">
+        <v>55</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="11">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
@@ -2913,33 +2960,36 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:20">
+    <row r="35" s="3" customFormat="1" spans="1:22">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F35" s="10">
+        <v>55</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="11">
         <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
-        <v>15000</v>
-      </c>
-      <c r="K35" s="11">
-        <v>3000</v>
-      </c>
-      <c r="M35" s="11">
-        <v>3000</v>
-      </c>
-      <c r="O35" s="11">
+        <v>18000</v>
+      </c>
+      <c r="K35" s="12">
+        <v>3000</v>
+      </c>
+      <c r="M35" s="12">
+        <v>3000</v>
+      </c>
+      <c r="O35" s="12">
         <v>3000</v>
       </c>
       <c r="Q35" s="3">
         <v>3000</v>
       </c>
-      <c r="T35" s="11">
+      <c r="T35" s="12">
+        <v>3000</v>
+      </c>
+      <c r="V35" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -2948,12 +2998,12 @@
         <v>34</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="10">
+        <v>55</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="11">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
@@ -2969,28 +3019,28 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="10">
+        <v>55</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="11">
         <f t="shared" si="2"/>
         <v>12000</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="12">
         <v>3000</v>
       </c>
       <c r="K37" s="3">
         <v>3000</v>
       </c>
-      <c r="P37" s="11">
-        <v>3000</v>
-      </c>
-      <c r="U37" s="11">
+      <c r="P37" s="12">
+        <v>3000</v>
+      </c>
+      <c r="U37" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -2998,33 +3048,36 @@
       <c r="A38" s="3">
         <v>36</v>
       </c>
+      <c r="C38" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D38" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" s="10">
+        <v>55</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="11">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="U38" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="39" s="3" customFormat="1" spans="1:21">
+      <c r="U38" s="12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" s="3" customFormat="1" spans="1:22">
       <c r="A39" s="3">
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F39" s="10">
+        <v>55</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="11">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="I39" s="3">
         <v>2000</v>
@@ -3036,6 +3089,9 @@
         <v>2000</v>
       </c>
       <c r="U39" s="3">
+        <v>2000</v>
+      </c>
+      <c r="V39" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3044,12 +3100,12 @@
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F40" s="10">
+        <v>55</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="11">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3068,12 +3124,12 @@
         <v>8210095108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="10">
+        <v>55</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="11">
         <f t="shared" si="2"/>
         <v>21000</v>
       </c>
@@ -3101,12 +3157,12 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42" s="10">
+        <v>55</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="11">
         <f t="shared" si="2"/>
         <v>1300</v>
       </c>
@@ -3119,12 +3175,12 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43" s="10">
+        <v>55</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3134,12 +3190,12 @@
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="10">
+        <v>55</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="11">
         <f t="shared" si="2"/>
         <v>15000</v>
       </c>
@@ -3159,27 +3215,30 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" s="3" customFormat="1" spans="1:15">
+    <row r="45" s="3" customFormat="1" spans="1:22">
       <c r="A45" s="3">
         <v>43</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="10">
+        <v>71</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" s="11">
         <f t="shared" si="2"/>
-        <v>12000</v>
-      </c>
-      <c r="J45" s="11">
+        <v>15000</v>
+      </c>
+      <c r="J45" s="12">
         <v>6000</v>
       </c>
-      <c r="M45" s="11">
+      <c r="M45" s="12">
         <v>3000</v>
       </c>
       <c r="O45" s="3">
+        <v>3000</v>
+      </c>
+      <c r="V45" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -3188,12 +3247,12 @@
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F46" s="10">
+      <c r="E46" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" s="11">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
@@ -3212,15 +3271,15 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="10">
+        <v>71</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" s="11">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
@@ -3228,27 +3287,27 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:19">
+    <row r="48" s="3" customFormat="1" spans="1:22">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="10">
+        <v>71</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="11">
         <f t="shared" si="2"/>
-        <v>11000</v>
-      </c>
-      <c r="L48" s="11">
+        <v>12000</v>
+      </c>
+      <c r="L48" s="12">
         <v>6000</v>
       </c>
       <c r="Q48" s="3">
@@ -3256,6 +3315,9 @@
       </c>
       <c r="S48" s="3">
         <v>2000</v>
+      </c>
+      <c r="V48" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:18">
@@ -3263,25 +3325,25 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F49" s="10">
+        <v>71</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="11">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="J49" s="11">
-        <v>3000</v>
-      </c>
-      <c r="M49" s="11">
+      <c r="J49" s="12">
+        <v>3000</v>
+      </c>
+      <c r="M49" s="12">
         <v>3000</v>
       </c>
       <c r="R49" s="3">
@@ -3293,15 +3355,15 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="10">
+        <v>71</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="11">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3317,12 +3379,12 @@
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="10">
+        <v>71</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" s="11">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
@@ -3333,27 +3395,27 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:19">
+    <row r="52" s="3" customFormat="1" spans="1:22">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F52" s="10">
+        <v>71</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="11">
         <f t="shared" si="2"/>
-        <v>11000</v>
-      </c>
-      <c r="H52" s="11">
-        <v>3000</v>
-      </c>
-      <c r="I52" s="11">
+        <v>14000</v>
+      </c>
+      <c r="H52" s="12">
+        <v>3000</v>
+      </c>
+      <c r="I52" s="12">
         <v>3000</v>
       </c>
       <c r="M52" s="3">
@@ -3368,8 +3430,11 @@
       <c r="S52" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="53" s="3" customFormat="1" spans="1:17">
+      <c r="V52" s="12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="1" spans="1:22">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3377,19 +3442,19 @@
         <v>6202424016</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="10">
+        <v>71</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="11">
         <f t="shared" si="2"/>
-        <v>5000</v>
-      </c>
-      <c r="J53" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M53" s="11">
+        <v>7000</v>
+      </c>
+      <c r="J53" s="12">
+        <v>2000</v>
+      </c>
+      <c r="M53" s="12">
         <v>1000</v>
       </c>
       <c r="O53" s="3">
@@ -3397,6 +3462,9 @@
       </c>
       <c r="Q53" s="3">
         <v>1000</v>
+      </c>
+      <c r="V53" s="12">
+        <v>2000</v>
       </c>
     </row>
     <row r="54" s="3" customFormat="1" spans="1:21">
@@ -3407,12 +3475,12 @@
         <v>7004211364</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" s="10">
+        <v>86</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="11">
         <f t="shared" si="2"/>
         <v>6000</v>
       </c>
@@ -3428,25 +3496,25 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F55" s="10">
+      <c r="E55" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" s="11">
         <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
       </c>
-      <c r="M55" s="11">
-        <v>5000</v>
-      </c>
-      <c r="S55" s="11">
+      <c r="M55" s="12">
+        <v>5000</v>
+      </c>
+      <c r="S55" s="12">
         <v>5000</v>
       </c>
       <c r="U55" s="3">
@@ -3458,12 +3526,12 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" s="10">
+        <v>86</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="11">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3475,36 +3543,39 @@
       </c>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" s="3" customFormat="1" spans="1:21">
+    <row r="57" s="3" customFormat="1" spans="1:22">
       <c r="A57" s="3">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C57" s="3">
         <v>9504958065</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="10">
+        <v>92</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="11">
         <f t="shared" si="2"/>
-        <v>20000</v>
-      </c>
-      <c r="H57" s="11">
+        <v>25000</v>
+      </c>
+      <c r="H57" s="12">
         <v>5000</v>
       </c>
       <c r="K57" s="3">
         <v>5000</v>
       </c>
-      <c r="N57" s="11">
-        <v>5000</v>
-      </c>
-      <c r="U57" s="11">
+      <c r="N57" s="12">
+        <v>5000</v>
+      </c>
+      <c r="U57" s="12">
+        <v>5000</v>
+      </c>
+      <c r="V57" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -3513,22 +3584,25 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F58" s="10">
+      <c r="E58" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="11">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="I58" s="11">
-        <v>5000</v>
-      </c>
-      <c r="U58" s="11">
+      <c r="I58" s="12">
+        <v>5000</v>
+      </c>
+      <c r="U58" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -3537,31 +3611,31 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="10">
+        <v>98</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="11">
         <f t="shared" si="2"/>
         <v>11000</v>
       </c>
-      <c r="G59" s="11">
+      <c r="G59" s="12">
         <v>2000</v>
       </c>
       <c r="K59" s="3">
         <v>3000</v>
       </c>
-      <c r="N59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="P59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="S59" s="11">
+      <c r="N59" s="12">
+        <v>2000</v>
+      </c>
+      <c r="P59" s="12">
+        <v>2000</v>
+      </c>
+      <c r="S59" s="12">
         <v>2000</v>
       </c>
     </row>
@@ -3570,12 +3644,12 @@
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" s="10">
+        <v>100</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="11">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3591,12 +3665,12 @@
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F61" s="10">
+        <v>102</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F61" s="11">
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
@@ -3612,12 +3686,12 @@
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F62" s="10">
+        <v>102</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F62" s="11">
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
@@ -3639,12 +3713,12 @@
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E63" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F63" s="10">
+      <c r="E63" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" s="11">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3660,12 +3734,12 @@
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="F64" s="10">
+        <v>102</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="11">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
@@ -3678,12 +3752,12 @@
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F65" s="10">
+        <v>102</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F65" s="11">
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
@@ -3708,12 +3782,12 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F66" s="10">
+        <v>102</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F66" s="11">
         <f t="shared" si="2"/>
         <v>15000</v>
       </c>
@@ -3726,37 +3800,40 @@
       <c r="R66" s="3">
         <v>3000</v>
       </c>
-      <c r="U66" s="11">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:18">
+      <c r="U66" s="12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:22">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C67" s="3">
         <v>8825370430</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F67" s="10">
+        <v>102</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67" s="11">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
-        <v>8000</v>
-      </c>
-      <c r="J67" s="11">
+        <v>10000</v>
+      </c>
+      <c r="J67" s="12">
         <v>4000</v>
       </c>
       <c r="N67" s="3">
         <v>2000</v>
       </c>
-      <c r="R67" s="11">
+      <c r="R67" s="12">
+        <v>2000</v>
+      </c>
+      <c r="V67" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3765,12 +3842,12 @@
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F68" s="10">
+        <v>102</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F68" s="11">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
@@ -3783,18 +3860,18 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C69" s="3">
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F69" s="10">
+        <v>113</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="11">
         <f t="shared" si="3"/>
         <v>7700</v>
       </c>
@@ -3813,7 +3890,7 @@
       <c r="Q69" s="3">
         <v>500</v>
       </c>
-      <c r="U69" s="11">
+      <c r="U69" s="12">
         <v>2100</v>
       </c>
       <c r="AE69" s="3"/>
@@ -3823,15 +3900,15 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F70" s="10">
+      <c r="E70" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F70" s="11">
         <f t="shared" si="3"/>
         <v>15000</v>
       </c>
@@ -3844,10 +3921,10 @@
       <c r="O70" s="3">
         <v>3000</v>
       </c>
-      <c r="R70" s="11">
-        <v>3000</v>
-      </c>
-      <c r="U70" s="11">
+      <c r="R70" s="12">
+        <v>3000</v>
+      </c>
+      <c r="U70" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -3856,15 +3933,15 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F71" s="10">
+        <v>113</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F71" s="11">
         <f t="shared" si="3"/>
         <v>12000</v>
       </c>
@@ -3874,10 +3951,10 @@
       <c r="L71" s="3">
         <v>2000</v>
       </c>
-      <c r="N71" s="11">
-        <v>2000</v>
-      </c>
-      <c r="Q71" s="11">
+      <c r="N71" s="12">
+        <v>2000</v>
+      </c>
+      <c r="Q71" s="12">
         <v>2000</v>
       </c>
       <c r="S71" s="3">
@@ -3891,10 +3968,10 @@
       <c r="A72" s="3">
         <v>70</v>
       </c>
-      <c r="E72" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F72" s="10">
+      <c r="E72" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F72" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3904,19 +3981,22 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F73" s="10">
+        <v>122</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F73" s="11">
         <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-      <c r="L73" s="11">
+      <c r="L73" s="12">
         <v>3000</v>
       </c>
     </row>
@@ -3924,10 +4004,10 @@
       <c r="A74" s="3">
         <v>72</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F74" s="10">
+      <c r="E74" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F74" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3937,16 +4017,16 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F75" s="10">
+        <v>125</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F75" s="11">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="M75" s="11">
+      <c r="M75" s="12">
         <v>2000</v>
       </c>
       <c r="U75" s="3">
@@ -3957,29 +4037,35 @@
       <c r="A76" s="3">
         <v>74</v>
       </c>
-      <c r="E76" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F76" s="10">
+      <c r="E76" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F76" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" s="3" customFormat="1" spans="1:12">
+    <row r="77" s="3" customFormat="1" spans="1:22">
       <c r="A77" s="3">
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F77" s="10">
+        <v>35</v>
+      </c>
+      <c r="C77" s="3">
+        <v>7004210181</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="11">
         <f t="shared" si="3"/>
-        <v>2000</v>
-      </c>
-      <c r="L77" s="11">
+        <v>4000</v>
+      </c>
+      <c r="L77" s="12">
+        <v>2000</v>
+      </c>
+      <c r="V77" s="12">
         <v>2000</v>
       </c>
     </row>
@@ -3988,16 +4074,16 @@
         <v>76</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F78" s="10">
+        <v>71</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F78" s="11">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
-      <c r="N78" s="11">
+      <c r="N78" s="12">
         <v>2000</v>
       </c>
     </row>
@@ -4005,10 +4091,13 @@
       <c r="A79" s="3">
         <v>77</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F79" s="10">
+      <c r="C79" s="3">
+        <v>9852299192</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F79" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4018,67 +4107,76 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F80" s="10">
+        <v>71</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F80" s="11">
         <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-      <c r="S80" s="11">
-        <v>2000</v>
-      </c>
-      <c r="U80" s="11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="81" s="3" customFormat="1" spans="1:11">
+      <c r="S80" s="12">
+        <v>2000</v>
+      </c>
+      <c r="U80" s="12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="81" s="3" customFormat="1" spans="1:22">
       <c r="A81" s="3">
         <v>79</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F81" s="10">
+        <v>133</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F81" s="11">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="K81" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="82" s="3" customFormat="1" spans="1:19">
+      <c r="V81" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="82" s="3" customFormat="1" spans="1:22">
       <c r="A82" s="3">
         <v>80</v>
       </c>
+      <c r="B82" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="D82" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F82" s="10">
+        <v>136</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F82" s="11">
         <f t="shared" si="3"/>
-        <v>20000</v>
-      </c>
-      <c r="H82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="K82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="P82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="S82" s="11">
+        <v>25000</v>
+      </c>
+      <c r="H82" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K82" s="12">
+        <v>5000</v>
+      </c>
+      <c r="P82" s="12">
+        <v>5000</v>
+      </c>
+      <c r="S82" s="12">
+        <v>5000</v>
+      </c>
+      <c r="V82" s="12">
         <v>5000</v>
       </c>
     </row>
@@ -4086,10 +4184,10 @@
       <c r="A83" s="3">
         <v>81</v>
       </c>
-      <c r="E83" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F83" s="10">
+      <c r="E83" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F83" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4098,10 +4196,10 @@
       <c r="A84" s="3">
         <v>82</v>
       </c>
-      <c r="E84" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F84" s="10">
+      <c r="E84" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F84" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4111,15 +4209,18 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E85" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F85" s="10">
+      <c r="E85" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F85" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4128,10 +4229,10 @@
       <c r="A86" s="3">
         <v>84</v>
       </c>
-      <c r="E86" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F86" s="10">
+      <c r="E86" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4140,10 +4241,10 @@
       <c r="A87" s="3">
         <v>85</v>
       </c>
-      <c r="E87" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F87" s="10">
+      <c r="E87" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F87" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4152,10 +4253,10 @@
       <c r="A88" s="3">
         <v>86</v>
       </c>
-      <c r="E88" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F88" s="10">
+      <c r="E88" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F88" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4164,10 +4265,10 @@
       <c r="A89" s="3">
         <v>87</v>
       </c>
-      <c r="E89" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F89" s="10">
+      <c r="E89" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F89" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4176,10 +4277,10 @@
       <c r="A90" s="3">
         <v>88</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F90" s="10">
+      <c r="E90" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F90" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4188,10 +4289,10 @@
       <c r="A91" s="3">
         <v>89</v>
       </c>
-      <c r="E91" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F91" s="10">
+      <c r="E91" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F91" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4200,10 +4301,16 @@
       <c r="A92" s="3">
         <v>90</v>
       </c>
-      <c r="E92" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F92" s="10">
+      <c r="C92" s="3">
+        <v>9631378928</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F92" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4212,10 +4319,10 @@
       <c r="A93" s="3">
         <v>91</v>
       </c>
-      <c r="E93" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F93" s="10">
+      <c r="E93" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F93" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4224,10 +4331,10 @@
       <c r="A94" s="3">
         <v>92</v>
       </c>
-      <c r="E94" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F94" s="10">
+      <c r="E94" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F94" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4237,22 +4344,25 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
+      </c>
+      <c r="C95" s="3">
+        <v>7004399486</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F95" s="10">
+        <v>153</v>
+      </c>
+      <c r="F95" s="11">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="K95" s="11">
-        <v>2000</v>
-      </c>
-      <c r="P95" s="11">
+      <c r="K95" s="12">
+        <v>2000</v>
+      </c>
+      <c r="P95" s="12">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 19 Jan 9PM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -42,6 +42,29 @@
           <t xml:space="preserve">
 5000-Digital
 5000-Cash</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+2000-Cash
+9000-Digital</t>
         </r>
       </text>
     </comment>
@@ -212,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="156">
   <si>
     <t>S.No.</t>
   </si>
@@ -319,283 +342,289 @@
     <t>SINGH COMMUNICATION(660315658)</t>
   </si>
   <si>
+    <t>Ajay 9939757903</t>
+  </si>
+  <si>
+    <t>ASHU COMMUNICATION(661025161)</t>
+  </si>
+  <si>
+    <t>ANIL PAN DUKAN(661705269)</t>
+  </si>
+  <si>
+    <t>Aarti 9523733118</t>
+  </si>
+  <si>
+    <t>MAA VINDHWASHNI COMMUNICATION(660301564)</t>
+  </si>
+  <si>
+    <t>MUKESH PAN BHANDAR(661613669)</t>
+  </si>
+  <si>
+    <t>Rajnish Kr 9708003669</t>
+  </si>
+  <si>
+    <t>Maa Bhindwashni Mobile Center(660587310)</t>
+  </si>
+  <si>
+    <t>Shantnu Kr.</t>
+  </si>
+  <si>
+    <t>MS RIYA ENTERPRISES(661562283)</t>
+  </si>
+  <si>
+    <t>ANKIT MOBILE CENTRE(661025000)</t>
+  </si>
+  <si>
+    <t>Sahaj Vasudha Kendra(660624994)</t>
+  </si>
+  <si>
+    <t>rangoli singar general store(660604869)</t>
+  </si>
+  <si>
+    <t>SUBODH PAN(661562286)</t>
+  </si>
+  <si>
+    <t>Nitish Kr.</t>
+  </si>
+  <si>
+    <t>GUPTA PAN DUKAN(661063901)</t>
+  </si>
+  <si>
+    <t>Basant Kr.</t>
+  </si>
+  <si>
+    <t>SUMAN PHONE GHAR(660315655)</t>
+  </si>
+  <si>
+    <t>BAJRANG MOBILE ELECTRIC &amp; ELEC(661591707)</t>
+  </si>
+  <si>
+    <t>Binay Lal</t>
+  </si>
+  <si>
+    <t>WALIDAD</t>
+  </si>
+  <si>
+    <t>ALL THE BEST COMMUNICATION(661096390)</t>
+  </si>
+  <si>
+    <t>NOKIA REPAIRING CENTER(660301577)</t>
+  </si>
+  <si>
+    <t>PRINCE COMMUNICATION(660831270)</t>
+  </si>
+  <si>
+    <t>Vicky Communication(660614434)</t>
+  </si>
+  <si>
+    <t>Kaler Electronics(660628532)</t>
+  </si>
+  <si>
+    <t>Sonu Kr.</t>
+  </si>
+  <si>
+    <t>MS OM COMPUTER(661542289)</t>
+  </si>
+  <si>
+    <t>8709954402/6207783075</t>
+  </si>
+  <si>
+    <t>SANTU KIRANA STORE(661752211)</t>
+  </si>
+  <si>
+    <t>ujjwal pustak bhandar(660849999)</t>
+  </si>
+  <si>
+    <t>PAYAL COMMNICATION(661644712)</t>
+  </si>
+  <si>
+    <t>PRAVEEN ELECTRONICS(660831267)</t>
+  </si>
+  <si>
+    <t>SONU PHONEX(661752239)</t>
+  </si>
+  <si>
+    <t>BHUMIKA ELECTRONICS(660320662)</t>
+  </si>
+  <si>
+    <t>CHANDAN TELECOM(661644693)</t>
+  </si>
+  <si>
+    <t>Deepak 7004687745</t>
+  </si>
+  <si>
+    <t>USRI</t>
+  </si>
+  <si>
+    <t>MEDIA MOBILE GALLERY(660315675)</t>
+  </si>
+  <si>
+    <t>PAWAN PAY PHONE(660297502)</t>
+  </si>
+  <si>
+    <t>Ranjit Kr.</t>
+  </si>
+  <si>
+    <t>KUMAR INTERNET(660322625)</t>
+  </si>
+  <si>
+    <t>Sanjeev Kr.</t>
+  </si>
+  <si>
+    <t>PRITI MOBILE CENTRE(660297509)</t>
+  </si>
+  <si>
+    <t>Vikash Kr.</t>
+  </si>
+  <si>
+    <t>PATEL TELECOM(661644686)</t>
+  </si>
+  <si>
+    <t>Chandan</t>
+  </si>
+  <si>
+    <t>KRISH RAJ MOBILE &amp; ELECTRONIC(661032970)</t>
+  </si>
+  <si>
+    <t>UTKARSH ENTERPRISES(661673664)</t>
+  </si>
+  <si>
+    <t>Akhilesh</t>
+  </si>
+  <si>
+    <t>DIVYANKA MOBILE CENTER(660315660)</t>
+  </si>
+  <si>
+    <t>Neha Phonex(660614432)</t>
+  </si>
+  <si>
+    <t>PARASI</t>
+  </si>
+  <si>
+    <t>ANISH MOBILE CENTER(661474493)</t>
+  </si>
+  <si>
+    <t>Navin Kr. Ojha</t>
+  </si>
+  <si>
+    <t>SINGH ENTERPRISES(660865703)</t>
+  </si>
+  <si>
+    <t>KALER ENTERPRISES(661674410)</t>
+  </si>
+  <si>
+    <t>Ranjit Kr. 9504958065</t>
+  </si>
+  <si>
+    <t>BADRABAD</t>
+  </si>
+  <si>
+    <t>ANJALI MOBILE RAMPURCHAE(661735620)</t>
+  </si>
+  <si>
+    <t>Amresh Kr.</t>
+  </si>
+  <si>
+    <t>9931812966/9572985032</t>
+  </si>
+  <si>
+    <t>MAA VINDHYAVASINI MOBILE CENTE(660064218)</t>
+  </si>
+  <si>
+    <t>D.K.</t>
+  </si>
+  <si>
+    <t>ITWA</t>
+  </si>
+  <si>
+    <t>chintu electronics(662114680)</t>
+  </si>
+  <si>
+    <t>NIRANJANPUR</t>
+  </si>
+  <si>
+    <t>RAJESH TELECOM(661613671)</t>
+  </si>
+  <si>
+    <t>CHANDA</t>
+  </si>
+  <si>
+    <t>MAA TELECOM(661361714)</t>
+  </si>
+  <si>
+    <t>RAJU TELECOM(661673669)</t>
+  </si>
+  <si>
+    <t>satyam mobile(661811583)</t>
+  </si>
+  <si>
+    <t>ARYANS PRINTER REPAIRING CENTE(662074228)</t>
+  </si>
+  <si>
+    <t>SHASHI PAY PHONE(661176231)</t>
+  </si>
+  <si>
+    <t>SANDEEP TELECOM(661066825)</t>
+  </si>
+  <si>
+    <t>Rajiv Kr/ Rajeev Kamal</t>
+  </si>
+  <si>
+    <t>SHRI SAI ELECTRONICS(661673670)</t>
+  </si>
+  <si>
+    <t>RAJESH TELECOM &amp; KIRANA DUKAN(661063895)</t>
+  </si>
+  <si>
+    <t>Brajesh Kr.</t>
+  </si>
+  <si>
+    <t>BELSAR</t>
+  </si>
+  <si>
+    <t>NISHA GENERAL STORE(661644683)</t>
+  </si>
+  <si>
+    <t>Chandan Kr</t>
+  </si>
+  <si>
+    <t>PRAKASH GENERAL SRINGAR STORE(661303685)</t>
+  </si>
+  <si>
+    <t>Sunil Kr./Gudiya</t>
+  </si>
+  <si>
+    <t>ANAND SRINGAR STORE(660831268)</t>
+  </si>
+  <si>
+    <t>ROHIT SHOE STORE(661670729)</t>
+  </si>
+  <si>
+    <t>INDRJEET KUMAR</t>
+  </si>
+  <si>
+    <t>8789783884/7061621223</t>
+  </si>
+  <si>
+    <t>Dhewai</t>
+  </si>
+  <si>
+    <t>maa phone ghar(662077151)</t>
+  </si>
+  <si>
+    <t>Payal Communication(660614430)</t>
+  </si>
+  <si>
+    <t>KAMTA</t>
+  </si>
+  <si>
+    <t>GRAMOTHAN SEVA KENDRA(661705272)</t>
+  </si>
+  <si>
+    <t>Rounk Mobile and Electronics(660584652)</t>
+  </si>
+  <si>
     <t>Ajay Kr.</t>
-  </si>
-  <si>
-    <t>ASHU COMMUNICATION(661025161)</t>
-  </si>
-  <si>
-    <t>ANIL PAN DUKAN(661705269)</t>
-  </si>
-  <si>
-    <t>Aarti 9523733118</t>
-  </si>
-  <si>
-    <t>MAA VINDHWASHNI COMMUNICATION(660301564)</t>
-  </si>
-  <si>
-    <t>MUKESH PAN BHANDAR(661613669)</t>
-  </si>
-  <si>
-    <t>Rajnish Kr 9708003669</t>
-  </si>
-  <si>
-    <t>Maa Bhindwashni Mobile Center(660587310)</t>
-  </si>
-  <si>
-    <t>Shantnu Kr.</t>
-  </si>
-  <si>
-    <t>MS RIYA ENTERPRISES(661562283)</t>
-  </si>
-  <si>
-    <t>ANKIT MOBILE CENTRE(661025000)</t>
-  </si>
-  <si>
-    <t>Sahaj Vasudha Kendra(660624994)</t>
-  </si>
-  <si>
-    <t>rangoli singar general store(660604869)</t>
-  </si>
-  <si>
-    <t>SUBODH PAN(661562286)</t>
-  </si>
-  <si>
-    <t>Nitish Kr.</t>
-  </si>
-  <si>
-    <t>GUPTA PAN DUKAN(661063901)</t>
-  </si>
-  <si>
-    <t>Basant Kr.</t>
-  </si>
-  <si>
-    <t>SUMAN PHONE GHAR(660315655)</t>
-  </si>
-  <si>
-    <t>BAJRANG MOBILE ELECTRIC &amp; ELEC(661591707)</t>
-  </si>
-  <si>
-    <t>Binay Lal</t>
-  </si>
-  <si>
-    <t>WALIDAD</t>
-  </si>
-  <si>
-    <t>ALL THE BEST COMMUNICATION(661096390)</t>
-  </si>
-  <si>
-    <t>NOKIA REPAIRING CENTER(660301577)</t>
-  </si>
-  <si>
-    <t>PRINCE COMMUNICATION(660831270)</t>
-  </si>
-  <si>
-    <t>Vicky Communication(660614434)</t>
-  </si>
-  <si>
-    <t>Kaler Electronics(660628532)</t>
-  </si>
-  <si>
-    <t>Sonu Kr.</t>
-  </si>
-  <si>
-    <t>MS OM COMPUTER(661542289)</t>
-  </si>
-  <si>
-    <t>8709954402/6207783075</t>
-  </si>
-  <si>
-    <t>SANTU KIRANA STORE(661752211)</t>
-  </si>
-  <si>
-    <t>ujjwal pustak bhandar(660849999)</t>
-  </si>
-  <si>
-    <t>PAYAL COMMNICATION(661644712)</t>
-  </si>
-  <si>
-    <t>PRAVEEN ELECTRONICS(660831267)</t>
-  </si>
-  <si>
-    <t>SONU PHONEX(661752239)</t>
-  </si>
-  <si>
-    <t>BHUMIKA ELECTRONICS(660320662)</t>
-  </si>
-  <si>
-    <t>CHANDAN TELECOM(661644693)</t>
-  </si>
-  <si>
-    <t>USRI</t>
-  </si>
-  <si>
-    <t>MEDIA MOBILE GALLERY(660315675)</t>
-  </si>
-  <si>
-    <t>PAWAN PAY PHONE(660297502)</t>
-  </si>
-  <si>
-    <t>Ranjit Kr.</t>
-  </si>
-  <si>
-    <t>KUMAR INTERNET(660322625)</t>
-  </si>
-  <si>
-    <t>Sanjeev Kr.</t>
-  </si>
-  <si>
-    <t>PRITI MOBILE CENTRE(660297509)</t>
-  </si>
-  <si>
-    <t>Vikash Kr.</t>
-  </si>
-  <si>
-    <t>PATEL TELECOM(661644686)</t>
-  </si>
-  <si>
-    <t>Chandan</t>
-  </si>
-  <si>
-    <t>KRISH RAJ MOBILE &amp; ELECTRONIC(661032970)</t>
-  </si>
-  <si>
-    <t>UTKARSH ENTERPRISES(661673664)</t>
-  </si>
-  <si>
-    <t>Akhilesh</t>
-  </si>
-  <si>
-    <t>DIVYANKA MOBILE CENTER(660315660)</t>
-  </si>
-  <si>
-    <t>Neha Phonex(660614432)</t>
-  </si>
-  <si>
-    <t>PARASI</t>
-  </si>
-  <si>
-    <t>ANISH MOBILE CENTER(661474493)</t>
-  </si>
-  <si>
-    <t>Navin Kr. Ojha</t>
-  </si>
-  <si>
-    <t>SINGH ENTERPRISES(660865703)</t>
-  </si>
-  <si>
-    <t>KALER ENTERPRISES(661674410)</t>
-  </si>
-  <si>
-    <t>Ranjit Kr. 9504958065</t>
-  </si>
-  <si>
-    <t>BADRABAD</t>
-  </si>
-  <si>
-    <t>ANJALI MOBILE RAMPURCHAE(661735620)</t>
-  </si>
-  <si>
-    <t>Amresh Kr.</t>
-  </si>
-  <si>
-    <t>9931812966/9572985032</t>
-  </si>
-  <si>
-    <t>MAA VINDHYAVASINI MOBILE CENTE(660064218)</t>
-  </si>
-  <si>
-    <t>D.K.</t>
-  </si>
-  <si>
-    <t>ITWA</t>
-  </si>
-  <si>
-    <t>chintu electronics(662114680)</t>
-  </si>
-  <si>
-    <t>NIRANJANPUR</t>
-  </si>
-  <si>
-    <t>RAJESH TELECOM(661613671)</t>
-  </si>
-  <si>
-    <t>CHANDA</t>
-  </si>
-  <si>
-    <t>MAA TELECOM(661361714)</t>
-  </si>
-  <si>
-    <t>RAJU TELECOM(661673669)</t>
-  </si>
-  <si>
-    <t>satyam mobile(661811583)</t>
-  </si>
-  <si>
-    <t>ARYANS PRINTER REPAIRING CENTE(662074228)</t>
-  </si>
-  <si>
-    <t>SHASHI PAY PHONE(661176231)</t>
-  </si>
-  <si>
-    <t>SANDEEP TELECOM(661066825)</t>
-  </si>
-  <si>
-    <t>Rajiv Kr/ Rajeev Kamal</t>
-  </si>
-  <si>
-    <t>SHRI SAI ELECTRONICS(661673670)</t>
-  </si>
-  <si>
-    <t>RAJESH TELECOM &amp; KIRANA DUKAN(661063895)</t>
-  </si>
-  <si>
-    <t>Brajesh Kr.</t>
-  </si>
-  <si>
-    <t>BELSAR</t>
-  </si>
-  <si>
-    <t>NISHA GENERAL STORE(661644683)</t>
-  </si>
-  <si>
-    <t>Chandan Kr</t>
-  </si>
-  <si>
-    <t>PRAKASH GENERAL SRINGAR STORE(661303685)</t>
-  </si>
-  <si>
-    <t>Sunil Kr.</t>
-  </si>
-  <si>
-    <t>ANAND SRINGAR STORE(660831268)</t>
-  </si>
-  <si>
-    <t>ROHIT SHOE STORE(661670729)</t>
-  </si>
-  <si>
-    <t>INDRJEET KUMAR</t>
-  </si>
-  <si>
-    <t>8789783884/7061621223</t>
-  </si>
-  <si>
-    <t>Dhewai</t>
-  </si>
-  <si>
-    <t>maa phone ghar(662077151)</t>
-  </si>
-  <si>
-    <t>Payal Communication(660614430)</t>
-  </si>
-  <si>
-    <t>KAMTA</t>
-  </si>
-  <si>
-    <t>GRAMOTHAN SEVA KENDRA(661705272)</t>
-  </si>
-  <si>
-    <t>Rounk Mobile and Electronics(660584652)</t>
   </si>
   <si>
     <t>SANGAM ENTERPRISES(661591706)</t>
@@ -681,11 +710,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -704,16 +733,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,6 +771,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -735,7 +796,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -749,32 +825,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -787,17 +840,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -813,29 +857,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -843,6 +865,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,25 +921,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,13 +945,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,13 +963,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -964,109 +1095,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,80 +1112,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1183,15 +1138,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1209,131 +1238,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1351,10 +1380,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1718,11 +1744,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="M38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="S76" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1741,132 +1767,132 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:37">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="5">
         <v>44197</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="5">
         <v>44198</v>
       </c>
-      <c r="I1" s="6">
+      <c r="I1" s="5">
         <v>44199</v>
       </c>
-      <c r="J1" s="6">
+      <c r="J1" s="5">
         <v>44200</v>
       </c>
-      <c r="K1" s="6">
+      <c r="K1" s="5">
         <v>44201</v>
       </c>
-      <c r="L1" s="6">
+      <c r="L1" s="5">
         <v>44202</v>
       </c>
-      <c r="M1" s="6">
+      <c r="M1" s="5">
         <v>44203</v>
       </c>
-      <c r="N1" s="6">
+      <c r="N1" s="5">
         <v>44204</v>
       </c>
-      <c r="O1" s="6">
+      <c r="O1" s="5">
         <v>44205</v>
       </c>
-      <c r="P1" s="6">
+      <c r="P1" s="5">
         <v>44206</v>
       </c>
-      <c r="Q1" s="6">
+      <c r="Q1" s="5">
         <v>44207</v>
       </c>
-      <c r="R1" s="6">
+      <c r="R1" s="5">
         <v>44208</v>
       </c>
-      <c r="S1" s="6">
+      <c r="S1" s="5">
         <v>44209</v>
       </c>
-      <c r="T1" s="6">
+      <c r="T1" s="5">
         <v>44210</v>
       </c>
-      <c r="U1" s="6">
+      <c r="U1" s="5">
         <v>44211</v>
       </c>
-      <c r="V1" s="6">
+      <c r="V1" s="5">
         <v>44212</v>
       </c>
-      <c r="W1" s="6">
+      <c r="W1" s="5">
         <v>44213</v>
       </c>
-      <c r="X1" s="6">
+      <c r="X1" s="5">
         <v>44214</v>
       </c>
-      <c r="Y1" s="6">
+      <c r="Y1" s="5">
         <v>44215</v>
       </c>
-      <c r="Z1" s="6">
+      <c r="Z1" s="5">
         <v>44216</v>
       </c>
-      <c r="AA1" s="6">
+      <c r="AA1" s="5">
         <v>44217</v>
       </c>
-      <c r="AB1" s="6">
+      <c r="AB1" s="5">
         <v>44218</v>
       </c>
-      <c r="AC1" s="6">
+      <c r="AC1" s="5">
         <v>44219</v>
       </c>
-      <c r="AD1" s="6">
+      <c r="AD1" s="5">
         <v>44220</v>
       </c>
-      <c r="AE1" s="6">
+      <c r="AE1" s="5">
         <v>44221</v>
       </c>
-      <c r="AF1" s="6">
+      <c r="AF1" s="5">
         <v>44222</v>
       </c>
-      <c r="AG1" s="6">
+      <c r="AG1" s="5">
         <v>44223</v>
       </c>
-      <c r="AH1" s="6">
+      <c r="AH1" s="5">
         <v>44224</v>
       </c>
-      <c r="AI1" s="6">
+      <c r="AI1" s="5">
         <v>44225</v>
       </c>
-      <c r="AJ1" s="6">
+      <c r="AJ1" s="5">
         <v>44226</v>
       </c>
-      <c r="AK1" s="6">
+      <c r="AK1" s="5">
         <v>44227</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:37">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>713000</v>
-      </c>
-      <c r="E2" s="9" t="s">
+        <v>850850</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>713000</v>
+        <v>850850</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1934,15 +1960,15 @@
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72150</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64700</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="0"/>
@@ -1993,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="1" spans="1:13">
+    <row r="3" s="3" customFormat="1" spans="1:24">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2006,45 +2032,51 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F34" si="1">SUM(G3:AK3)</f>
-        <v>6000</v>
-      </c>
-      <c r="H3" s="12">
-        <v>3000</v>
-      </c>
-      <c r="M3" s="12">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="1" spans="1:17">
+        <v>9000</v>
+      </c>
+      <c r="H3" s="11">
+        <v>3000</v>
+      </c>
+      <c r="M3" s="11">
+        <v>3000</v>
+      </c>
+      <c r="X3" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="1" spans="1:25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" si="1"/>
+        <v>3500</v>
+      </c>
+      <c r="Q4" s="11">
         <v>1500</v>
       </c>
-      <c r="Q4" s="12">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="1" spans="1:18">
+      <c r="Y4" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:24">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2054,12 +2086,12 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>8500</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
@@ -2076,8 +2108,11 @@
       <c r="R5" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:21">
+      <c r="X5" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2090,30 +2125,36 @@
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>13000</v>
-      </c>
-      <c r="H6" s="12">
+        <v>18000</v>
+      </c>
+      <c r="H6" s="11">
         <v>3000</v>
       </c>
       <c r="M6" s="3">
         <v>2000</v>
       </c>
-      <c r="Q6" s="12">
-        <v>3000</v>
-      </c>
-      <c r="R6" s="12">
+      <c r="Q6" s="11">
+        <v>3000</v>
+      </c>
+      <c r="R6" s="11">
         <v>2000</v>
       </c>
       <c r="U6" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:18">
+      <c r="X6" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Y6" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2123,27 +2164,30 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>25000</v>
-      </c>
-      <c r="J7" s="12">
+        <v>36000</v>
+      </c>
+      <c r="J7" s="11">
         <v>4000</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>7000</v>
       </c>
       <c r="N7" s="3">
         <v>4000</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="11">
         <v>10000</v>
       </c>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:12">
+      <c r="Y7" s="11">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:24">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2153,14 +2197,17 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X8" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2174,10 +2221,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2188,7 +2235,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:21">
+    <row r="10" s="3" customFormat="1" spans="1:25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2198,12 +2245,12 @@
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="K10" s="3">
         <v>5000</v>
@@ -2217,8 +2264,14 @@
       <c r="U10" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="11" s="3" customFormat="1" spans="1:18">
+      <c r="X10" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" s="3" customFormat="1" spans="1:25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2231,37 +2284,40 @@
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="L11" s="11">
+        <v>2000</v>
+      </c>
+      <c r="R11" s="11">
+        <v>4000</v>
+      </c>
+      <c r="Y11" s="11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7004923653</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="10">
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
-      <c r="L11" s="12">
-        <v>2000</v>
-      </c>
-      <c r="R11" s="12">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:21">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4">
-        <v>7004923653</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
       <c r="I12" s="3">
         <v>1000</v>
       </c>
@@ -2283,8 +2339,11 @@
       <c r="U12" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:21">
+      <c r="Y12" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:24">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2294,12 +2353,12 @@
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="I13" s="3">
         <v>5000</v>
@@ -2310,8 +2369,11 @@
       <c r="U13" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:22">
+      <c r="X13" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2324,12 +2386,12 @@
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>31000</v>
+        <v>37000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2337,7 +2399,7 @@
       <c r="I14" s="3">
         <v>2500</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <v>1500</v>
       </c>
       <c r="K14" s="3">
@@ -2346,7 +2408,7 @@
       <c r="L14" s="3">
         <v>2500</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="11">
         <v>1500</v>
       </c>
       <c r="N14" s="3">
@@ -2355,7 +2417,7 @@
       <c r="O14" s="3">
         <v>2500</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="11">
         <v>2500</v>
       </c>
       <c r="R14" s="3">
@@ -2370,8 +2432,14 @@
       <c r="V14" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:21">
+      <c r="X14" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2382,12 +2450,12 @@
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="M15" s="3">
         <v>2000</v>
@@ -2395,8 +2463,11 @@
       <c r="U15" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="Y15" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2409,12 +2480,12 @@
       <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="H16" s="3">
         <v>500</v>
@@ -2422,8 +2493,11 @@
       <c r="J16" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="17" s="3" customFormat="1" spans="1:19">
+      <c r="Y16" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="1" spans="1:25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2436,12 +2510,12 @@
       <c r="D17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <f t="shared" si="1"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H17" s="3">
         <v>3000</v>
@@ -2454,6 +2528,9 @@
       </c>
       <c r="S17" s="3">
         <v>3500</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:22">
@@ -2466,10 +2543,10 @@
       <c r="D18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
@@ -2479,7 +2556,7 @@
       <c r="N18" s="3">
         <v>5000</v>
       </c>
-      <c r="V18" s="12">
+      <c r="V18" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -2496,21 +2573,21 @@
       <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="L19" s="12">
-        <v>2000</v>
-      </c>
-      <c r="P19" s="12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" s="3" customFormat="1" spans="1:17">
+      <c r="L19" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P19" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" s="3" customFormat="1" spans="1:24">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2520,12 +2597,12 @@
       <c r="D20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J20" s="3">
         <v>2000</v>
@@ -2533,8 +2610,11 @@
       <c r="Q20" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" s="3" customFormat="1" spans="1:18">
+      <c r="X20" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" s="3" customFormat="1" spans="1:25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2547,24 +2627,27 @@
       <c r="D21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
-      </c>
-      <c r="H21" s="12">
-        <v>5000</v>
-      </c>
-      <c r="M21" s="12">
-        <v>5000</v>
-      </c>
-      <c r="R21" s="12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="1" spans="1:22">
+        <v>20000</v>
+      </c>
+      <c r="H21" s="11">
+        <v>5000</v>
+      </c>
+      <c r="M21" s="11">
+        <v>5000</v>
+      </c>
+      <c r="R21" s="11">
+        <v>5000</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:24">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2574,12 +2657,12 @@
       <c r="D22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="H22" s="3">
         <v>1000</v>
@@ -2596,8 +2679,11 @@
       <c r="V22" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" s="3" customFormat="1" spans="1:21">
+      <c r="X22" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:24">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2610,20 +2696,23 @@
       <c r="D23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>9000</v>
-      </c>
-      <c r="P23" s="12">
+        <v>12000</v>
+      </c>
+      <c r="P23" s="11">
         <v>3000</v>
       </c>
       <c r="R23" s="3">
         <v>3000</v>
       </c>
       <c r="U23" s="3">
+        <v>3000</v>
+      </c>
+      <c r="X23" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2640,27 +2729,27 @@
       <c r="D24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="H24" s="12">
-        <v>5000</v>
-      </c>
-      <c r="J24" s="12">
-        <v>5000</v>
-      </c>
-      <c r="O24" s="12">
-        <v>5000</v>
-      </c>
-      <c r="T24" s="12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="25" s="3" customFormat="1" spans="1:22">
+      <c r="H24" s="11">
+        <v>5000</v>
+      </c>
+      <c r="J24" s="11">
+        <v>5000</v>
+      </c>
+      <c r="O24" s="11">
+        <v>5000</v>
+      </c>
+      <c r="T24" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="1" spans="1:24">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2670,17 +2759,17 @@
       <c r="D25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>17500</v>
+        <v>20500</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="11">
         <v>3000</v>
       </c>
       <c r="N25" s="3">
@@ -2695,8 +2784,11 @@
       <c r="V25" s="3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="26" s="3" customFormat="1" spans="1:21">
+      <c r="X25" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" spans="1:24">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2706,12 +2798,12 @@
       <c r="D26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>6950</v>
       </c>
       <c r="H26" s="3">
         <v>1000</v>
@@ -2727,6 +2819,9 @@
       </c>
       <c r="U26" s="3">
         <v>1000</v>
+      </c>
+      <c r="X26" s="3">
+        <v>1950</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" spans="1:21">
@@ -2739,10 +2834,10 @@
       <c r="D27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2763,10 +2858,10 @@
       <c r="D28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2777,7 +2872,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="29" s="3" customFormat="1" spans="1:18">
+    <row r="29" s="3" customFormat="1" spans="1:25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2787,21 +2882,24 @@
       <c r="D29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="M29" s="12">
-        <v>5000</v>
-      </c>
-      <c r="R29" s="12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="30" s="3" customFormat="1" spans="1:21">
+        <v>15000</v>
+      </c>
+      <c r="M29" s="11">
+        <v>5000</v>
+      </c>
+      <c r="R29" s="11">
+        <v>5000</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" s="3" customFormat="1" spans="1:24">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2811,45 +2909,48 @@
       <c r="D30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="10">
         <f t="shared" si="1"/>
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="H30" s="3">
         <v>10000</v>
       </c>
-      <c r="K30" s="12">
-        <v>5000</v>
-      </c>
-      <c r="M30" s="12">
-        <v>5000</v>
-      </c>
-      <c r="P30" s="12">
-        <v>5000</v>
-      </c>
-      <c r="S30" s="12">
-        <v>5000</v>
-      </c>
-      <c r="U30" s="12">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="31" s="3" customFormat="1" spans="1:21">
+      <c r="K30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="M30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="P30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U30" s="11">
+        <v>5000</v>
+      </c>
+      <c r="X30" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" s="3" customFormat="1" spans="1:25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -2867,6 +2968,9 @@
         <v>500</v>
       </c>
       <c r="U31" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Y31" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2880,20 +2984,20 @@
       <c r="D32" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="10">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="H32" s="3">
         <v>1000</v>
       </c>
-      <c r="M32" s="12">
-        <v>1000</v>
-      </c>
-      <c r="Q32" s="12">
+      <c r="M32" s="11">
+        <v>1000</v>
+      </c>
+      <c r="Q32" s="11">
         <v>2000</v>
       </c>
       <c r="V32" s="3">
@@ -2907,10 +3011,10 @@
       <c r="D33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="10">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
@@ -2927,7 +3031,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="1" spans="1:21">
+    <row r="34" s="3" customFormat="1" spans="1:24">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2937,12 +3041,12 @@
       <c r="D34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="H34" s="3">
         <v>1000</v>
@@ -2957,6 +3061,9 @@
         <v>1000</v>
       </c>
       <c r="U34" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X34" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2967,29 +3074,29 @@
       <c r="D35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="10">
         <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
         <v>18000</v>
       </c>
-      <c r="K35" s="12">
-        <v>3000</v>
-      </c>
-      <c r="M35" s="12">
-        <v>3000</v>
-      </c>
-      <c r="O35" s="12">
+      <c r="K35" s="11">
+        <v>3000</v>
+      </c>
+      <c r="M35" s="11">
+        <v>3000</v>
+      </c>
+      <c r="O35" s="11">
         <v>3000</v>
       </c>
       <c r="Q35" s="3">
         <v>3000</v>
       </c>
-      <c r="T35" s="12">
-        <v>3000</v>
-      </c>
-      <c r="V35" s="12">
+      <c r="T35" s="11">
+        <v>3000</v>
+      </c>
+      <c r="V35" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -3000,10 +3107,10 @@
       <c r="D36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="10">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
@@ -3024,23 +3131,23 @@
       <c r="D37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="10">
         <f t="shared" si="2"/>
         <v>12000</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="11">
         <v>3000</v>
       </c>
       <c r="K37" s="3">
         <v>3000</v>
       </c>
-      <c r="P37" s="12">
-        <v>3000</v>
-      </c>
-      <c r="U37" s="12">
+      <c r="P37" s="11">
+        <v>3000</v>
+      </c>
+      <c r="U37" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -3048,36 +3155,36 @@
       <c r="A38" s="3">
         <v>36</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="10">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="U38" s="12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="39" s="3" customFormat="1" spans="1:22">
+      <c r="U38" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" s="3" customFormat="1" spans="1:24">
       <c r="A39" s="3">
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="I39" s="3">
         <v>2000</v>
@@ -3094,80 +3201,92 @@
       <c r="V39" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="40" s="3" customFormat="1" spans="1:18">
+      <c r="X39" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="40" s="3" customFormat="1" spans="1:25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="10">
+        <f t="shared" si="2"/>
+        <v>6000</v>
+      </c>
+      <c r="H40" s="3">
+        <v>2000</v>
+      </c>
+      <c r="R40" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Y40" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="41" s="3" customFormat="1" spans="1:25">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="C41" s="3">
+        <v>8210095108</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="10">
+        <f t="shared" si="2"/>
+        <v>24000</v>
+      </c>
+      <c r="H41" s="3">
+        <v>6000</v>
+      </c>
+      <c r="K41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="N41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="S41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="42" s="3" customFormat="1" spans="1:25">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="10">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
-      <c r="H40" s="3">
-        <v>2000</v>
-      </c>
-      <c r="R40" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="41" s="3" customFormat="1" spans="1:21">
-      <c r="A41" s="3">
-        <v>39</v>
-      </c>
-      <c r="C41" s="3">
-        <v>8210095108</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" s="11">
-        <f t="shared" si="2"/>
-        <v>21000</v>
-      </c>
-      <c r="H41" s="3">
-        <v>6000</v>
-      </c>
-      <c r="K41" s="3">
-        <v>3000</v>
-      </c>
-      <c r="N41" s="3">
-        <v>3000</v>
-      </c>
-      <c r="Q41" s="3">
-        <v>3000</v>
-      </c>
-      <c r="S41" s="3">
-        <v>3000</v>
-      </c>
-      <c r="U41" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="42" s="3" customFormat="1" spans="1:8">
-      <c r="A42" s="3">
-        <v>40</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="11">
-        <f t="shared" si="2"/>
-        <v>1300</v>
-      </c>
       <c r="H42" s="3">
         <v>1300</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>2700</v>
       </c>
     </row>
     <row r="43" s="3" customFormat="1" spans="1:6">
@@ -3177,27 +3296,27 @@
       <c r="D43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:19">
+    <row r="44" s="3" customFormat="1" spans="1:24">
       <c r="A44" s="3">
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H44" s="3">
         <v>3000</v>
@@ -3214,47 +3333,56 @@
       <c r="S44" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="45" s="3" customFormat="1" spans="1:22">
+      <c r="X44" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" s="3" customFormat="1" spans="1:25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D45" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E45" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F45" s="11">
+      <c r="E45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
-      </c>
-      <c r="J45" s="12">
+        <v>18000</v>
+      </c>
+      <c r="J45" s="11">
         <v>6000</v>
       </c>
-      <c r="M45" s="12">
+      <c r="M45" s="11">
         <v>3000</v>
       </c>
       <c r="O45" s="3">
         <v>3000</v>
       </c>
-      <c r="V45" s="12">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="46" s="3" customFormat="1" spans="1:17">
+      <c r="V45" s="11">
+        <v>3000</v>
+      </c>
+      <c r="Y45" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="46" s="3" customFormat="1" spans="1:24">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F46" s="11">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="I46" s="3">
         <v>3000</v>
@@ -3265,49 +3393,55 @@
       <c r="Q46" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="47" s="3" customFormat="1" spans="1:15">
+      <c r="X46" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="47" s="3" customFormat="1" spans="1:24">
       <c r="A47" s="3">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F47" s="11">
+        <v>72</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F47" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="O47" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="48" s="3" customFormat="1" spans="1:22">
+      <c r="X47" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="48" s="3" customFormat="1" spans="1:25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F48" s="11">
+        <v>72</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
-      </c>
-      <c r="L48" s="12">
+        <v>13500</v>
+      </c>
+      <c r="L48" s="11">
         <v>6000</v>
       </c>
       <c r="Q48" s="3">
@@ -3319,58 +3453,70 @@
       <c r="V48" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="49" s="3" customFormat="1" spans="1:18">
+      <c r="Y48" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" s="3" customFormat="1" spans="1:25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" s="11">
+        <v>72</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F49" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
-      </c>
-      <c r="J49" s="12">
-        <v>3000</v>
-      </c>
-      <c r="M49" s="12">
+        <v>18000</v>
+      </c>
+      <c r="J49" s="11">
+        <v>3000</v>
+      </c>
+      <c r="M49" s="11">
         <v>3000</v>
       </c>
       <c r="R49" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="50" s="3" customFormat="1" spans="1:15">
+      <c r="X49" s="11">
+        <v>6000</v>
+      </c>
+      <c r="Y49" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="50" s="3" customFormat="1" spans="1:24">
       <c r="A50" s="3">
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F50" s="11">
+        <v>72</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I50" s="3">
         <v>2000</v>
       </c>
       <c r="O50" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X50" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3379,12 +3525,12 @@
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F51" s="11">
+        <v>72</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="10">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
@@ -3395,27 +3541,27 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:22">
+    <row r="52" s="3" customFormat="1" spans="1:24">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="11">
+        <v>72</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>14000</v>
-      </c>
-      <c r="H52" s="12">
-        <v>3000</v>
-      </c>
-      <c r="I52" s="12">
+        <v>15000</v>
+      </c>
+      <c r="H52" s="11">
+        <v>3000</v>
+      </c>
+      <c r="I52" s="11">
         <v>3000</v>
       </c>
       <c r="M52" s="3">
@@ -3430,11 +3576,14 @@
       <c r="S52" s="3">
         <v>1000</v>
       </c>
-      <c r="V52" s="12">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="53" s="3" customFormat="1" spans="1:22">
+      <c r="V52" s="11">
+        <v>3000</v>
+      </c>
+      <c r="X52" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="1" spans="1:25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3442,19 +3591,19 @@
         <v>6202424016</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="11">
+        <v>72</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="10">
         <f t="shared" si="2"/>
-        <v>7000</v>
-      </c>
-      <c r="J53" s="12">
-        <v>2000</v>
-      </c>
-      <c r="M53" s="12">
+        <v>10000</v>
+      </c>
+      <c r="J53" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M53" s="11">
         <v>1000</v>
       </c>
       <c r="O53" s="3">
@@ -3463,8 +3612,11 @@
       <c r="Q53" s="3">
         <v>1000</v>
       </c>
-      <c r="V53" s="12">
-        <v>2000</v>
+      <c r="V53" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Y53" s="11">
+        <v>3000</v>
       </c>
     </row>
     <row r="54" s="3" customFormat="1" spans="1:21">
@@ -3475,12 +3627,12 @@
         <v>7004211364</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="11">
+      <c r="E54" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" s="10">
         <f t="shared" si="2"/>
         <v>6000</v>
       </c>
@@ -3496,25 +3648,25 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F55" s="11">
+        <v>87</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="10">
         <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
       </c>
-      <c r="M55" s="12">
-        <v>5000</v>
-      </c>
-      <c r="S55" s="12">
+      <c r="M55" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S55" s="11">
         <v>5000</v>
       </c>
       <c r="U55" s="3">
@@ -3526,12 +3678,12 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F56" s="11">
+        <v>87</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" s="10">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3548,34 +3700,34 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C57" s="3">
         <v>9504958065</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E57" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F57" s="11">
+      <c r="E57" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F57" s="10">
         <f t="shared" si="2"/>
         <v>25000</v>
       </c>
-      <c r="H57" s="12">
+      <c r="H57" s="11">
         <v>5000</v>
       </c>
       <c r="K57" s="3">
         <v>5000</v>
       </c>
-      <c r="N57" s="12">
-        <v>5000</v>
-      </c>
-      <c r="U57" s="12">
-        <v>5000</v>
-      </c>
-      <c r="V57" s="12">
+      <c r="N57" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U57" s="11">
+        <v>5000</v>
+      </c>
+      <c r="V57" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -3584,25 +3736,25 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="14" t="s">
         <v>95</v>
       </c>
+      <c r="C58" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="D58" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="11">
+        <v>93</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" s="10">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="I58" s="12">
-        <v>5000</v>
-      </c>
-      <c r="U58" s="12">
+      <c r="I58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U58" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -3611,53 +3763,56 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E59" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="11">
+      <c r="E59" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F59" s="10">
         <f t="shared" si="2"/>
         <v>11000</v>
       </c>
-      <c r="G59" s="12">
+      <c r="G59" s="11">
         <v>2000</v>
       </c>
       <c r="K59" s="3">
         <v>3000</v>
       </c>
-      <c r="N59" s="12">
-        <v>2000</v>
-      </c>
-      <c r="P59" s="12">
-        <v>2000</v>
-      </c>
-      <c r="S59" s="12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="60" s="3" customFormat="1" spans="1:19">
+      <c r="N59" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P59" s="11">
+        <v>2000</v>
+      </c>
+      <c r="S59" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="60" s="3" customFormat="1" spans="1:24">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F60" s="11">
+      <c r="E60" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F60" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>5500</v>
       </c>
       <c r="I60" s="3">
         <v>2000</v>
       </c>
       <c r="S60" s="3">
         <v>2000</v>
+      </c>
+      <c r="X60" s="3">
+        <v>1500</v>
       </c>
     </row>
     <row r="61" s="3" customFormat="1" spans="1:21">
@@ -3665,12 +3820,12 @@
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E61" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="11">
+      <c r="E61" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" s="10">
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
@@ -3681,19 +3836,19 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="62" s="3" customFormat="1" spans="1:21">
+    <row r="62" s="3" customFormat="1" spans="1:24">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F62" s="11">
+        <v>103</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="10">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="H62" s="3">
         <v>2000</v>
@@ -3705,6 +3860,9 @@
         <v>2000</v>
       </c>
       <c r="U62" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X62" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3713,12 +3871,12 @@
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F63" s="11">
+        <v>103</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="10">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
@@ -3729,37 +3887,40 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="64" s="3" customFormat="1" spans="1:14">
+    <row r="64" s="3" customFormat="1" spans="1:24">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F64" s="11">
+        <v>103</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="10">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="N64" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="65" s="3" customFormat="1" spans="1:21">
+      <c r="X64" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65" s="3" customFormat="1" spans="1:24">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F65" s="11">
+        <v>103</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -3774,6 +3935,9 @@
         <v>10000</v>
       </c>
       <c r="U65" s="3">
+        <v>5000</v>
+      </c>
+      <c r="X65" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3782,12 +3946,12 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F66" s="11">
+        <v>103</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" s="10">
         <f t="shared" si="2"/>
         <v>15000</v>
       </c>
@@ -3800,40 +3964,43 @@
       <c r="R66" s="3">
         <v>3000</v>
       </c>
-      <c r="U66" s="12">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:22">
+      <c r="U66" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C67" s="3">
         <v>8825370430</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F67" s="11">
+        <v>103</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67" s="10">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
-        <v>10000</v>
-      </c>
-      <c r="J67" s="12">
+        <v>12000</v>
+      </c>
+      <c r="J67" s="11">
         <v>4000</v>
       </c>
       <c r="N67" s="3">
         <v>2000</v>
       </c>
-      <c r="R67" s="12">
+      <c r="R67" s="11">
         <v>2000</v>
       </c>
       <c r="V67" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Y67" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3842,12 +4009,12 @@
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F68" s="11">
+        <v>103</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F68" s="10">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
@@ -3860,20 +4027,20 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C69" s="3">
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E69" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="11">
+      <c r="E69" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F69" s="10">
         <f t="shared" si="3"/>
-        <v>7700</v>
+        <v>10400</v>
       </c>
       <c r="H69" s="3">
         <v>2800</v>
@@ -3890,27 +4057,33 @@
       <c r="Q69" s="3">
         <v>500</v>
       </c>
-      <c r="U69" s="12">
+      <c r="U69" s="11">
         <v>2100</v>
       </c>
+      <c r="X69" s="3">
+        <v>1200</v>
+      </c>
+      <c r="Y69" s="3">
+        <v>1500</v>
+      </c>
       <c r="AE69" s="3"/>
     </row>
-    <row r="70" s="3" customFormat="1" spans="1:21">
+    <row r="70" s="3" customFormat="1" spans="1:24">
       <c r="A70" s="3">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F70" s="11">
+        <v>114</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="10">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="I70" s="3">
         <v>3000</v>
@@ -3921,29 +4094,32 @@
       <c r="O70" s="3">
         <v>3000</v>
       </c>
-      <c r="R70" s="12">
-        <v>3000</v>
-      </c>
-      <c r="U70" s="12">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="71" s="3" customFormat="1" spans="1:21">
+      <c r="R70" s="11">
+        <v>3000</v>
+      </c>
+      <c r="U70" s="11">
+        <v>3000</v>
+      </c>
+      <c r="X70" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="71" s="3" customFormat="1" spans="1:24">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F71" s="11">
+        <v>114</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="H71" s="3">
         <v>2000</v>
@@ -3951,16 +4127,19 @@
       <c r="L71" s="3">
         <v>2000</v>
       </c>
-      <c r="N71" s="12">
-        <v>2000</v>
-      </c>
-      <c r="Q71" s="12">
+      <c r="N71" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Q71" s="11">
         <v>2000</v>
       </c>
       <c r="S71" s="3">
         <v>2000</v>
       </c>
       <c r="U71" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X71" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3968,10 +4147,10 @@
       <c r="A72" s="3">
         <v>70</v>
       </c>
-      <c r="E72" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F72" s="11">
+      <c r="E72" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3981,22 +4160,22 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C73" s="14" t="s">
         <v>121</v>
       </c>
+      <c r="C73" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="D73" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E73" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F73" s="11">
+      <c r="E73" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F73" s="10">
         <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-      <c r="L73" s="12">
+      <c r="L73" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -4004,10 +4183,10 @@
       <c r="A74" s="3">
         <v>72</v>
       </c>
-      <c r="E74" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F74" s="11">
+      <c r="E74" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F74" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4017,16 +4196,16 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E75" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F75" s="11">
+      <c r="E75" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" s="10">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="M75" s="12">
+      <c r="M75" s="11">
         <v>2000</v>
       </c>
       <c r="U75" s="3">
@@ -4037,10 +4216,10 @@
       <c r="A76" s="3">
         <v>74</v>
       </c>
-      <c r="E76" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F76" s="11">
+      <c r="E76" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F76" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4050,22 +4229,22 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="C77" s="3">
         <v>7004210181</v>
       </c>
-      <c r="E77" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F77" s="11">
+      <c r="E77" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F77" s="10">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="L77" s="12">
-        <v>2000</v>
-      </c>
-      <c r="V77" s="12">
+      <c r="L77" s="11">
+        <v>2000</v>
+      </c>
+      <c r="V77" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -4074,16 +4253,16 @@
         <v>76</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F78" s="11">
+        <v>72</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F78" s="10">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
-      <c r="N78" s="12">
+      <c r="N78" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -4094,35 +4273,38 @@
       <c r="C79" s="3">
         <v>9852299192</v>
       </c>
-      <c r="E79" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F79" s="11">
+      <c r="E79" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F79" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" s="3" customFormat="1" spans="1:21">
+    <row r="80" s="3" customFormat="1" spans="1:24">
       <c r="A80" s="3">
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F80" s="11">
+        <v>72</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F80" s="10">
         <f t="shared" si="3"/>
-        <v>3000</v>
-      </c>
-      <c r="S80" s="12">
-        <v>2000</v>
-      </c>
-      <c r="U80" s="12">
+        <v>4000</v>
+      </c>
+      <c r="S80" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U80" s="11">
+        <v>1000</v>
+      </c>
+      <c r="X80" s="11">
         <v>1000</v>
       </c>
     </row>
@@ -4131,12 +4313,12 @@
         <v>79</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F81" s="11">
+        <v>135</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F81" s="10">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
@@ -4152,31 +4334,31 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F82" s="11">
+        <v>138</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F82" s="10">
         <f t="shared" si="3"/>
         <v>25000</v>
       </c>
-      <c r="H82" s="12">
-        <v>5000</v>
-      </c>
-      <c r="K82" s="12">
-        <v>5000</v>
-      </c>
-      <c r="P82" s="12">
-        <v>5000</v>
-      </c>
-      <c r="S82" s="12">
-        <v>5000</v>
-      </c>
-      <c r="V82" s="12">
+      <c r="H82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="K82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="P82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="V82" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -4184,10 +4366,10 @@
       <c r="A83" s="3">
         <v>81</v>
       </c>
-      <c r="E83" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F83" s="11">
+      <c r="E83" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F83" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4196,10 +4378,10 @@
       <c r="A84" s="3">
         <v>82</v>
       </c>
-      <c r="E84" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F84" s="11">
+      <c r="E84" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F84" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4209,18 +4391,18 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F85" s="11">
+        <v>138</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F85" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4229,10 +4411,10 @@
       <c r="A86" s="3">
         <v>84</v>
       </c>
-      <c r="E86" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F86" s="11">
+      <c r="E86" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4241,10 +4423,10 @@
       <c r="A87" s="3">
         <v>85</v>
       </c>
-      <c r="E87" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F87" s="11">
+      <c r="E87" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F87" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4253,10 +4435,10 @@
       <c r="A88" s="3">
         <v>86</v>
       </c>
-      <c r="E88" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F88" s="11">
+      <c r="E88" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F88" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4265,10 +4447,10 @@
       <c r="A89" s="3">
         <v>87</v>
       </c>
-      <c r="E89" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F89" s="11">
+      <c r="E89" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F89" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4277,10 +4459,13 @@
       <c r="A90" s="3">
         <v>88</v>
       </c>
-      <c r="E90" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F90" s="11">
+      <c r="C90" s="3">
+        <v>9934079439</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4289,10 +4474,10 @@
       <c r="A91" s="3">
         <v>89</v>
       </c>
-      <c r="E91" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F91" s="11">
+      <c r="E91" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F91" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4305,12 +4490,12 @@
         <v>9631378928</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F92" s="11">
+        <v>103</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F92" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4319,10 +4504,10 @@
       <c r="A93" s="3">
         <v>91</v>
       </c>
-      <c r="E93" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F93" s="11">
+      <c r="E93" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F93" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4331,39 +4516,42 @@
       <c r="A94" s="3">
         <v>92</v>
       </c>
-      <c r="E94" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="F94" s="11">
+      <c r="E94" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F94" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:23">
       <c r="A95" s="3">
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C95" s="3">
         <v>7004399486</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F95" s="11">
+        <v>155</v>
+      </c>
+      <c r="F95" s="10">
         <f t="shared" si="3"/>
-        <v>4000</v>
-      </c>
-      <c r="K95" s="12">
-        <v>2000</v>
-      </c>
-      <c r="P95" s="12">
-        <v>2000</v>
+        <v>5000</v>
+      </c>
+      <c r="K95" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P95" s="11">
+        <v>2000</v>
+      </c>
+      <c r="W95" s="11">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated till 22 Jan 2AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -161,29 +161,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA56" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t>Vijay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t xml:space="preserve">
-1500-Cash
-500-Digital</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="U69" authorId="0">
       <text>
         <r>
@@ -235,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
   <si>
     <t>S.No.</t>
   </si>
@@ -711,9 +688,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -733,20 +710,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -755,9 +718,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,7 +735,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -790,21 +784,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -833,6 +812,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -847,9 +833,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -862,27 +854,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -921,19 +898,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,55 +946,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,7 +976,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1023,19 +1000,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1047,7 +1012,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,19 +1042,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,25 +1060,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1112,6 +1089,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1126,6 +1118,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1154,30 +1166,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1201,23 +1189,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1235,31 +1212,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1268,97 +1245,97 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1744,11 +1721,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="R17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="S48" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+      <selection pane="bottomRight" activeCell="AA67" sqref="AA67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1885,14 +1862,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>882850</v>
+        <v>935900</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>882850</v>
+        <v>935900</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1976,7 +1953,7 @@
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53050</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
@@ -2019,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="1" spans="1:24">
+    <row r="3" s="3" customFormat="1" spans="1:27">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2037,7 +2014,7 @@
       </c>
       <c r="F3" s="10">
         <f t="shared" ref="F3:F34" si="1">SUM(G3:AK3)</f>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="H3" s="11">
         <v>3000</v>
@@ -2046,6 +2023,9 @@
         <v>3000</v>
       </c>
       <c r="X3" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AA3" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -2211,7 +2191,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:21">
+    <row r="9" s="3" customFormat="1" spans="1:27">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2226,7 +2206,7 @@
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="K9" s="3">
         <v>2000</v>
@@ -2234,8 +2214,11 @@
       <c r="U9" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="10" s="3" customFormat="1" spans="1:25">
+      <c r="AA9" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="1" spans="1:27">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2250,7 +2233,7 @@
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="K10" s="3">
         <v>5000</v>
@@ -2269,6 +2252,9 @@
       </c>
       <c r="Y10" s="3">
         <v>2000</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:25">
@@ -2373,7 +2359,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:26">
+    <row r="14" s="3" customFormat="1" spans="1:27">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2391,7 +2377,7 @@
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>39000</v>
+        <v>40000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2440,6 +2426,9 @@
       </c>
       <c r="Z14" s="3">
         <v>2000</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:25">
@@ -2659,7 +2648,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:26">
+    <row r="22" s="3" customFormat="1" spans="1:27">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2674,7 +2663,7 @@
       </c>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="H22" s="3">
         <v>1000</v>
@@ -2695,6 +2684,9 @@
         <v>1000</v>
       </c>
       <c r="Z22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AA22" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -2809,7 +2801,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" s="3" customFormat="1" spans="1:24">
+    <row r="26" s="3" customFormat="1" spans="1:27">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2824,7 +2816,7 @@
       </c>
       <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>6950</v>
+        <v>8000</v>
       </c>
       <c r="H26" s="3">
         <v>1000</v>
@@ -2843,6 +2835,9 @@
       </c>
       <c r="X26" s="3">
         <v>1950</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>1050</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" spans="1:21">
@@ -2959,7 +2954,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:25">
+    <row r="31" s="3" customFormat="1" spans="1:27">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2971,7 +2966,7 @@
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -2992,6 +2987,9 @@
         <v>1000</v>
       </c>
       <c r="Y31" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AA31" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3055,7 +3053,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="1" spans="1:24">
+    <row r="34" s="3" customFormat="1" spans="1:27">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -3070,7 +3068,7 @@
       </c>
       <c r="F34" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="H34" s="3">
         <v>1000</v>
@@ -3088,6 +3086,9 @@
         <v>1000</v>
       </c>
       <c r="X34" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AA34" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3262,7 +3263,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:25">
+    <row r="41" s="3" customFormat="1" spans="1:27">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3277,7 +3278,7 @@
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="H41" s="3">
         <v>6000</v>
@@ -3298,6 +3299,9 @@
         <v>3000</v>
       </c>
       <c r="Y41" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AA41" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3337,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:24">
+    <row r="44" s="3" customFormat="1" spans="1:27">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3349,7 +3353,7 @@
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="H44" s="3">
         <v>3000</v>
@@ -3367,6 +3371,9 @@
         <v>3000</v>
       </c>
       <c r="X44" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AA44" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3655,7 +3662,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="54" s="3" customFormat="1" spans="1:21">
+    <row r="54" s="3" customFormat="1" spans="1:27">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3670,7 +3677,7 @@
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="L54" s="3">
         <v>4000</v>
@@ -3678,8 +3685,11 @@
       <c r="U54" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="55" s="3" customFormat="1" spans="1:21">
+      <c r="AA54" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="55" s="3" customFormat="1" spans="1:27">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -3694,7 +3704,7 @@
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
@@ -3706,6 +3716,9 @@
         <v>5000</v>
       </c>
       <c r="U55" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AA55" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -3721,7 +3734,7 @@
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="L56" s="3">
         <v>2000</v>
@@ -3729,7 +3742,9 @@
       <c r="U56" s="3">
         <v>2000</v>
       </c>
-      <c r="AA56" s="3"/>
+      <c r="AA56" s="3">
+        <v>2000</v>
+      </c>
     </row>
     <row r="57" s="3" customFormat="1" spans="1:22">
       <c r="A57" s="3">
@@ -3794,7 +3809,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="59" s="3" customFormat="1" spans="1:25">
+    <row r="59" s="3" customFormat="1" spans="1:27">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -3809,7 +3824,7 @@
       </c>
       <c r="F59" s="10">
         <f t="shared" si="2"/>
-        <v>13000</v>
+        <v>15000</v>
       </c>
       <c r="G59" s="11">
         <v>2000</v>
@@ -3827,6 +3842,9 @@
         <v>2000</v>
       </c>
       <c r="Y59" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AA59" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3980,7 +3998,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="66" s="3" customFormat="1" spans="1:21">
+    <row r="66" s="3" customFormat="1" spans="1:27">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3992,7 +4010,7 @@
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>21000</v>
       </c>
       <c r="H66" s="3">
         <v>3000</v>
@@ -4005,6 +4023,9 @@
       </c>
       <c r="U66" s="11">
         <v>3000</v>
+      </c>
+      <c r="AA66" s="3">
+        <v>6000</v>
       </c>
     </row>
     <row r="67" s="3" customFormat="1" spans="1:25">
@@ -4079,7 +4100,7 @@
       </c>
       <c r="F69" s="10">
         <f t="shared" si="3"/>
-        <v>10400</v>
+        <v>11400</v>
       </c>
       <c r="H69" s="3">
         <v>2800</v>
@@ -4104,6 +4125,9 @@
       </c>
       <c r="Y69" s="3">
         <v>1500</v>
+      </c>
+      <c r="AA69" s="3">
+        <v>1000</v>
       </c>
       <c r="AE69" s="3"/>
     </row>
@@ -4503,31 +4527,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" s="3" customFormat="1" spans="1:6">
+    <row r="90" s="3" customFormat="1" spans="1:27">
       <c r="A90" s="3">
         <v>88</v>
       </c>
       <c r="C90" s="3">
         <v>9934079439</v>
       </c>
+      <c r="D90" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="E90" s="9" t="s">
         <v>149</v>
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" s="3" customFormat="1" spans="1:6">
+        <v>5000</v>
+      </c>
+      <c r="AA90" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="91" s="3" customFormat="1" spans="1:27">
       <c r="A91" s="3">
         <v>89</v>
       </c>
+      <c r="D91" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E91" s="9" t="s">
         <v>150</v>
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5000</v>
+      </c>
+      <c r="AA91" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="92" s="3" customFormat="1" spans="1:6">
@@ -4572,7 +4608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:27">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -4590,7 +4626,7 @@
       </c>
       <c r="F95" s="10">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="K95" s="11">
         <v>2000</v>
@@ -4600,6 +4636,9 @@
       </c>
       <c r="W95" s="11">
         <v>1000</v>
+      </c>
+      <c r="AA95" s="11">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated till 23 Jan 9AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -65,6 +65,29 @@
           <t xml:space="preserve">
 2000-Cash
 9000-Digital</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1200-Cash
+800-Digital</t>
         </r>
       </text>
     </comment>
@@ -212,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="157">
   <si>
     <t>S.No.</t>
   </si>
@@ -313,6 +336,9 @@
     <t>Glaxy Mobile and Digital Studi(660587311)</t>
   </si>
   <si>
+    <t>Sailesh</t>
+  </si>
+  <si>
     <t>MAHENDIA</t>
   </si>
   <si>
@@ -397,7 +423,7 @@
     <t>Kaler Electronics(660628532)</t>
   </si>
   <si>
-    <t>Sonu Kr.</t>
+    <t>Sonu/Rupa 9708329918</t>
   </si>
   <si>
     <t>MS OM COMPUTER(661542289)</t>
@@ -687,11 +713,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -710,25 +736,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,22 +751,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -773,15 +796,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -811,15 +841,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -833,6 +864,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -840,26 +872,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -898,7 +924,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -910,43 +996,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,31 +1014,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,7 +1038,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,7 +1068,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,19 +1080,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,7 +1092,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,25 +1104,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,17 +1118,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1122,13 +1142,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1145,23 +1184,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1183,9 +1207,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1194,15 +1220,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1212,130 +1238,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1357,7 +1383,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1721,11 +1747,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="S48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="V20" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA67" sqref="AA67"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1862,14 +1888,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>935900</v>
+        <v>978400</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>935900</v>
+        <v>978400</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1953,11 +1979,11 @@
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>53050</v>
+        <v>55050</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40500</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
@@ -2134,7 +2160,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:25">
+    <row r="7" s="3" customFormat="1" spans="1:28">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2149,7 +2175,7 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>36000</v>
+        <v>38000</v>
       </c>
       <c r="J7" s="11">
         <v>4000</v>
@@ -2165,6 +2191,9 @@
       </c>
       <c r="Y7" s="11">
         <v>11000</v>
+      </c>
+      <c r="AB7" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:24">
@@ -2329,7 +2358,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="1" spans="1:24">
+    <row r="13" s="3" customFormat="1" spans="1:28">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2344,7 +2373,7 @@
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="I13" s="3">
         <v>5000</v>
@@ -2358,8 +2387,11 @@
       <c r="X13" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:27">
+      <c r="AB13" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:28">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2377,7 +2409,7 @@
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>42000</v>
       </c>
       <c r="H14" s="3">
         <v>2500</v>
@@ -2429,6 +2461,9 @@
       </c>
       <c r="AA14" s="3">
         <v>1000</v>
+      </c>
+      <c r="AB14" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:25">
@@ -2525,22 +2560,25 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="1" spans="1:22">
+    <row r="18" s="3" customFormat="1" spans="1:28">
       <c r="A18" s="3">
         <v>16</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C18" s="4">
         <v>9661555592</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F18" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="J18" s="3">
         <v>5000</v>
@@ -2549,6 +2587,9 @@
         <v>5000</v>
       </c>
       <c r="V18" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AB18" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -2557,16 +2598,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4">
         <v>8340523512</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
@@ -2593,10 +2634,10 @@
         <v>8825310472</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
@@ -2620,16 +2661,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" s="4">
         <v>7004478123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" s="10">
         <f t="shared" si="1"/>
@@ -2656,10 +2697,10 @@
         <v>7667895364</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
@@ -2695,16 +2736,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="4">
         <v>7006041121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
@@ -2728,16 +2769,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="4">
         <v>8709658240</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="1"/>
@@ -2759,7 +2800,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:26">
+    <row r="25" s="3" customFormat="1" spans="1:28">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2767,14 +2808,14 @@
         <v>8709612020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>21000</v>
+        <v>23000</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
@@ -2800,8 +2841,11 @@
       <c r="Z25" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="26" s="3" customFormat="1" spans="1:27">
+      <c r="AB25" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" spans="1:28">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2809,14 +2853,14 @@
         <v>9973040600</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="H26" s="3">
         <v>1000</v>
@@ -2839,8 +2883,11 @@
       <c r="AA26" s="3">
         <v>1050</v>
       </c>
-    </row>
-    <row r="27" s="3" customFormat="1" spans="1:21">
+      <c r="AB26" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" s="3" customFormat="1" spans="1:28">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2848,14 +2895,14 @@
         <v>9973345687</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H27" s="3">
         <v>2000</v>
@@ -2863,8 +2910,11 @@
       <c r="U27" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="28" s="3" customFormat="1" spans="1:14">
+      <c r="AB27" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="1" spans="1:28">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2872,19 +2922,22 @@
         <v>9631391206</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H28" s="3">
         <v>2000</v>
       </c>
       <c r="N28" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AB28" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2893,13 +2946,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F29" s="10">
         <f t="shared" si="1"/>
@@ -2920,13 +2973,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F30" s="10">
         <f t="shared" si="1"/>
@@ -2954,19 +3007,19 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:27">
+    <row r="31" s="3" customFormat="1" spans="1:28">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>7000</v>
+        <v>7500</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -2992,23 +3045,26 @@
       <c r="AA31" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="32" s="3" customFormat="1" spans="1:26">
+      <c r="AB31" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" s="3" customFormat="1" spans="1:28">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F32" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="H32" s="3">
         <v>1000</v>
@@ -3023,6 +3079,9 @@
         <v>1000</v>
       </c>
       <c r="Z32" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AB32" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3031,10 +3090,10 @@
         <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" si="1"/>
@@ -3061,10 +3120,10 @@
         <v>7654800030</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F34" s="10">
         <f t="shared" si="1"/>
@@ -3097,10 +3156,10 @@
         <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F35" s="10">
         <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
@@ -3133,10 +3192,10 @@
         <v>34</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="2"/>
@@ -3149,22 +3208,22 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="37" s="3" customFormat="1" spans="1:26">
+    <row r="37" s="3" customFormat="1" spans="1:28">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H37" s="11">
         <v>3000</v>
@@ -3179,6 +3238,9 @@
         <v>3000</v>
       </c>
       <c r="Z37" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AB37" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -3187,13 +3249,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
@@ -3208,10 +3270,10 @@
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F39" s="10">
         <f t="shared" si="2"/>
@@ -3244,10 +3306,10 @@
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F40" s="10">
         <f t="shared" si="2"/>
@@ -3271,10 +3333,10 @@
         <v>8210095108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
@@ -3310,10 +3372,10 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F42" s="10">
         <f t="shared" si="2"/>
@@ -3331,10 +3393,10 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F43" s="10">
         <f t="shared" si="2"/>
@@ -3346,10 +3408,10 @@
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
@@ -3382,13 +3444,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F45" s="10">
         <f t="shared" si="2"/>
@@ -3415,10 +3477,10 @@
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F46" s="10">
         <f t="shared" si="2"/>
@@ -3442,13 +3504,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F47" s="10">
         <f t="shared" si="2"/>
@@ -3466,16 +3528,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
@@ -3505,16 +3567,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F49" s="10">
         <f t="shared" si="2"/>
@@ -3541,13 +3603,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F50" s="10">
         <f t="shared" si="2"/>
@@ -3568,10 +3630,10 @@
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F51" s="10">
         <f t="shared" si="2"/>
@@ -3584,22 +3646,22 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:24">
+    <row r="52" s="3" customFormat="1" spans="1:27">
       <c r="A52" s="3">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>17000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -3624,6 +3686,9 @@
       </c>
       <c r="X52" s="3">
         <v>1000</v>
+      </c>
+      <c r="AA52" s="11">
+        <v>2000</v>
       </c>
     </row>
     <row r="53" s="3" customFormat="1" spans="1:25">
@@ -3634,10 +3699,10 @@
         <v>6202424016</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F53" s="10">
         <f t="shared" si="2"/>
@@ -3670,10 +3735,10 @@
         <v>7004211364</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
@@ -3694,13 +3759,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
@@ -3727,10 +3792,10 @@
         <v>54</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
@@ -3746,25 +3811,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="57" s="3" customFormat="1" spans="1:22">
+    <row r="57" s="3" customFormat="1" spans="1:28">
       <c r="A57" s="3">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C57" s="3">
         <v>9504958065</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F57" s="10">
         <f t="shared" si="2"/>
-        <v>25000</v>
+        <v>35000</v>
       </c>
       <c r="H57" s="11">
         <v>5000</v>
@@ -3780,6 +3845,9 @@
       </c>
       <c r="V57" s="11">
         <v>5000</v>
+      </c>
+      <c r="AB57" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="58" s="3" customFormat="1" spans="1:21">
@@ -3787,16 +3855,16 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F58" s="10">
         <f t="shared" si="2"/>
@@ -3809,22 +3877,22 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="59" s="3" customFormat="1" spans="1:27">
+    <row r="59" s="3" customFormat="1" spans="1:28">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F59" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>17000</v>
       </c>
       <c r="G59" s="11">
         <v>2000</v>
@@ -3845,6 +3913,9 @@
         <v>2000</v>
       </c>
       <c r="AA59" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AB59" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3853,10 +3924,10 @@
         <v>58</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F60" s="10">
         <f t="shared" si="2"/>
@@ -3877,10 +3948,10 @@
         <v>59</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F61" s="10">
         <f t="shared" si="2"/>
@@ -3898,10 +3969,10 @@
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
@@ -3928,10 +3999,10 @@
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
@@ -3949,10 +4020,10 @@
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F64" s="10">
         <f t="shared" si="2"/>
@@ -3970,10 +4041,10 @@
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
@@ -4003,10 +4074,10 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
@@ -4033,16 +4104,16 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C67" s="3">
         <v>8825370430</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F67" s="10">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
@@ -4069,10 +4140,10 @@
         <v>66</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F68" s="10">
         <f t="shared" si="3"/>
@@ -4087,16 +4158,16 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C69" s="3">
         <v>6200769032</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F69" s="10">
         <f t="shared" si="3"/>
@@ -4136,13 +4207,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F70" s="10">
         <f t="shared" si="3"/>
@@ -4170,22 +4241,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="71" s="3" customFormat="1" spans="1:26">
+    <row r="71" s="3" customFormat="1" spans="1:28">
       <c r="A71" s="3">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>17000</v>
+        <v>19000</v>
       </c>
       <c r="H71" s="3">
         <v>2000</v>
@@ -4210,6 +4281,9 @@
       </c>
       <c r="Z71" s="11">
         <v>3000</v>
+      </c>
+      <c r="AB71" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="72" s="3" customFormat="1" spans="1:6">
@@ -4217,7 +4291,7 @@
         <v>70</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F72" s="10">
         <f t="shared" si="3"/>
@@ -4229,16 +4303,16 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
@@ -4253,7 +4327,7 @@
         <v>72</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F74" s="10">
         <f t="shared" si="3"/>
@@ -4265,10 +4339,10 @@
         <v>73</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F75" s="10">
         <f t="shared" si="3"/>
@@ -4286,7 +4360,7 @@
         <v>74</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F76" s="10">
         <f t="shared" si="3"/>
@@ -4298,13 +4372,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C77" s="3">
         <v>7004210181</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
@@ -4322,10 +4396,10 @@
         <v>76</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F78" s="10">
         <f t="shared" si="3"/>
@@ -4343,7 +4417,7 @@
         <v>9852299192</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F79" s="10">
         <f t="shared" si="3"/>
@@ -4355,13 +4429,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F80" s="10">
         <f t="shared" si="3"/>
@@ -4377,25 +4451,28 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="81" s="3" customFormat="1" spans="1:22">
+    <row r="81" s="3" customFormat="1" spans="1:28">
       <c r="A81" s="3">
         <v>79</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F81" s="10">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="K81" s="3">
         <v>2000</v>
       </c>
       <c r="V81" s="3">
         <v>3000</v>
+      </c>
+      <c r="AB81" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="82" s="3" customFormat="1" spans="1:22">
@@ -4403,13 +4480,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
@@ -4436,7 +4513,7 @@
         <v>81</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F83" s="10">
         <f t="shared" si="3"/>
@@ -4448,7 +4525,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F84" s="10">
         <f t="shared" si="3"/>
@@ -4460,16 +4537,16 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F85" s="10">
         <f t="shared" si="3"/>
@@ -4481,7 +4558,7 @@
         <v>84</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F86" s="10">
         <f t="shared" si="3"/>
@@ -4496,7 +4573,7 @@
         <v>9015378357</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F87" s="10">
         <f t="shared" si="3"/>
@@ -4508,7 +4585,7 @@
         <v>86</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F88" s="10">
         <f t="shared" si="3"/>
@@ -4520,7 +4597,7 @@
         <v>87</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F89" s="10">
         <f t="shared" si="3"/>
@@ -4535,10 +4612,10 @@
         <v>9934079439</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
@@ -4553,10 +4630,10 @@
         <v>89</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
@@ -4574,10 +4651,10 @@
         <v>9631378928</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F92" s="10">
         <f t="shared" si="3"/>
@@ -4589,7 +4666,7 @@
         <v>91</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F93" s="10">
         <f t="shared" si="3"/>
@@ -4601,7 +4678,7 @@
         <v>92</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F94" s="10">
         <f t="shared" si="3"/>
@@ -4613,16 +4690,16 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C95" s="3">
         <v>7004399486</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F95" s="10">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
data updated till 24 Jan 10AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -207,29 +207,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE69" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t>Vijay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t xml:space="preserve">
-2000-Digital
-200-Cash</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -330,7 +307,7 @@
     <t>Rohit Mobile Care-(662161247)</t>
   </si>
   <si>
-    <t>Ranveer</t>
+    <t>Ranveer/Rina</t>
   </si>
   <si>
     <t>Glaxy Mobile and Digital Studi(660587311)</t>
@@ -713,11 +690,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -737,6 +714,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -744,14 +728,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -766,7 +751,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -780,6 +773,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -787,31 +788,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,13 +827,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -864,9 +835,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -880,12 +850,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -924,19 +901,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,7 +937,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,25 +949,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,31 +961,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,7 +973,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,13 +1003,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1062,49 +1057,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1121,8 +1098,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1142,6 +1134,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1157,35 +1158,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1220,13 +1197,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1238,31 +1215,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,97 +1248,97 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1383,7 +1360,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1747,11 +1724,11 @@
   <dimension ref="A1:AK95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="V20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1761,7 +1738,7 @@
     <col min="3" max="3" width="11.7142857142857" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
     <col min="5" max="5" width="51.1428571428571" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6.57142857142857" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.57142857142857" style="4" customWidth="1"/>
     <col min="7" max="7" width="6.14285714285714" style="3" customWidth="1"/>
     <col min="8" max="8" width="6.57142857142857" style="3" customWidth="1"/>
     <col min="9" max="15" width="6.14285714285714" style="3" customWidth="1"/>
@@ -1888,14 +1865,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>978400</v>
+        <v>1045900</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>978400</v>
+        <v>1045900</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -1987,7 +1964,7 @@
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67500</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="0"/>
@@ -2160,7 +2137,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:28">
+    <row r="7" s="3" customFormat="1" spans="1:29">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2175,7 +2152,7 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>38000</v>
+        <v>46000</v>
       </c>
       <c r="J7" s="11">
         <v>4000</v>
@@ -2194,6 +2171,9 @@
       </c>
       <c r="AB7" s="11">
         <v>2000</v>
+      </c>
+      <c r="AC7" s="11">
+        <v>8000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:24">
@@ -2466,7 +2446,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="1" spans="1:25">
+    <row r="15" s="3" customFormat="1" spans="1:29">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2482,7 +2462,7 @@
       </c>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="M15" s="3">
         <v>2000</v>
@@ -2491,6 +2471,9 @@
         <v>2000</v>
       </c>
       <c r="Y15" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AC15" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -2524,7 +2507,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="1" spans="1:25">
+    <row r="17" s="3" customFormat="1" spans="1:29">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2542,7 +2525,7 @@
       </c>
       <c r="F17" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="H17" s="3">
         <v>3000</v>
@@ -2557,6 +2540,9 @@
         <v>3500</v>
       </c>
       <c r="Y17" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AC17" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -2593,7 +2579,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="1" spans="1:26">
+    <row r="19" s="3" customFormat="1" spans="1:29">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2611,7 +2597,7 @@
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="L19" s="11">
         <v>2000</v>
@@ -2623,6 +2609,9 @@
         <v>2000</v>
       </c>
       <c r="Z19" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AC19" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -2731,7 +2720,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" s="3" customFormat="1" spans="1:24">
+    <row r="23" s="3" customFormat="1" spans="1:29">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2749,7 +2738,7 @@
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="P23" s="11">
         <v>3000</v>
@@ -2761,6 +2750,9 @@
         <v>3000</v>
       </c>
       <c r="X23" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AC23" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2800,7 +2792,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:28">
+    <row r="25" s="3" customFormat="1" spans="1:29">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2815,7 +2807,7 @@
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>23000</v>
+        <v>24000</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
@@ -2843,6 +2835,9 @@
       </c>
       <c r="AB25" s="3">
         <v>2000</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" spans="1:28">
@@ -3007,7 +3002,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:28">
+    <row r="31" s="3" customFormat="1" spans="1:29">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -3019,7 +3014,7 @@
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -3046,6 +3041,9 @@
         <v>1000</v>
       </c>
       <c r="AB31" s="3">
+        <v>500</v>
+      </c>
+      <c r="AC31" s="3">
         <v>500</v>
       </c>
     </row>
@@ -3244,7 +3242,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="38" s="3" customFormat="1" spans="1:21">
+    <row r="38" s="3" customFormat="1" spans="1:29">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -3259,9 +3257,12 @@
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="U38" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AC38" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -3472,7 +3473,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:24">
+    <row r="46" s="3" customFormat="1" spans="1:29">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -3484,7 +3485,7 @@
       </c>
       <c r="F46" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>14300</v>
       </c>
       <c r="I46" s="3">
         <v>3000</v>
@@ -3497,6 +3498,9 @@
       </c>
       <c r="X46" s="3">
         <v>3000</v>
+      </c>
+      <c r="AC46" s="3">
+        <v>2300</v>
       </c>
     </row>
     <row r="47" s="3" customFormat="1" spans="1:24">
@@ -3523,7 +3527,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:26">
+    <row r="48" s="3" customFormat="1" spans="1:29">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3541,7 +3545,7 @@
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="L48" s="11">
         <v>6000</v>
@@ -3561,8 +3565,11 @@
       <c r="Z48" s="11">
         <v>1500</v>
       </c>
-    </row>
-    <row r="49" s="3" customFormat="1" spans="1:25">
+      <c r="AC48" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="49" s="3" customFormat="1" spans="1:29">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -3580,7 +3587,7 @@
       </c>
       <c r="F49" s="10">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="J49" s="11">
         <v>3000</v>
@@ -3595,6 +3602,9 @@
         <v>6000</v>
       </c>
       <c r="Y49" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AC49" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -3646,7 +3656,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:27">
+    <row r="52" s="3" customFormat="1" spans="1:29">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3661,7 +3671,7 @@
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>17000</v>
+        <v>18000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -3690,8 +3700,11 @@
       <c r="AA52" s="11">
         <v>2000</v>
       </c>
-    </row>
-    <row r="53" s="3" customFormat="1" spans="1:25">
+      <c r="AC52" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="1" spans="1:29">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3706,7 +3719,7 @@
       </c>
       <c r="F53" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="J53" s="11">
         <v>2000</v>
@@ -3725,6 +3738,9 @@
       </c>
       <c r="Y53" s="11">
         <v>3000</v>
+      </c>
+      <c r="AC53" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="54" s="3" customFormat="1" spans="1:27">
@@ -3754,7 +3770,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="55" s="3" customFormat="1" spans="1:27">
+    <row r="55" s="3" customFormat="1" spans="1:29">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -3769,7 +3785,7 @@
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
-        <v>25000</v>
+        <v>30500</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
@@ -3785,6 +3801,9 @@
       </c>
       <c r="AA55" s="3">
         <v>5000</v>
+      </c>
+      <c r="AC55" s="3">
+        <v>5500</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="1" spans="1:27">
@@ -3943,7 +3962,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="61" s="3" customFormat="1" spans="1:21">
+    <row r="61" s="3" customFormat="1" spans="1:29">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3955,12 +3974,15 @@
       </c>
       <c r="F61" s="10">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="N61" s="3">
         <v>4000</v>
       </c>
       <c r="U61" s="3">
+        <v>4000</v>
+      </c>
+      <c r="AC61" s="3">
         <v>4000</v>
       </c>
     </row>
@@ -3994,7 +4016,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" s="3" customFormat="1" spans="1:21">
+    <row r="63" s="3" customFormat="1" spans="1:29">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -4006,12 +4028,15 @@
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="L63" s="3">
         <v>2000</v>
       </c>
       <c r="U63" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AC63" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -4036,7 +4061,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:24">
+    <row r="65" s="3" customFormat="1" spans="1:29">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -4048,7 +4073,7 @@
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -4066,6 +4091,9 @@
         <v>5000</v>
       </c>
       <c r="X65" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AC65" s="3">
         <v>5000</v>
       </c>
     </row>
@@ -4099,7 +4127,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="67" s="3" customFormat="1" spans="1:25">
+    <row r="67" s="3" customFormat="1" spans="1:29">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -4117,7 +4145,7 @@
       </c>
       <c r="F67" s="10">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="J67" s="11">
         <v>4000</v>
@@ -4134,8 +4162,11 @@
       <c r="Y67" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="68" s="3" customFormat="1" spans="1:8">
+      <c r="AC67" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="68" s="3" customFormat="1" spans="1:29">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -4147,13 +4178,16 @@
       </c>
       <c r="F68" s="10">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>1700</v>
       </c>
       <c r="H68" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="69" s="3" customFormat="1" spans="1:31">
+      <c r="AC68" s="3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="1" spans="1:27">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -4200,9 +4234,8 @@
       <c r="AA69" s="3">
         <v>1000</v>
       </c>
-      <c r="AE69" s="3"/>
-    </row>
-    <row r="70" s="3" customFormat="1" spans="1:26">
+    </row>
+    <row r="70" s="3" customFormat="1" spans="1:29">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -4217,7 +4250,7 @@
       </c>
       <c r="F70" s="10">
         <f t="shared" si="3"/>
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="I70" s="3">
         <v>3000</v>
@@ -4238,6 +4271,9 @@
         <v>3000</v>
       </c>
       <c r="Z70" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AC70" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -4367,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" s="3" customFormat="1" spans="1:22">
+    <row r="77" s="3" customFormat="1" spans="1:29">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -4382,7 +4418,7 @@
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="L77" s="11">
         <v>2000</v>
@@ -4390,8 +4426,11 @@
       <c r="V77" s="11">
         <v>2000</v>
       </c>
-    </row>
-    <row r="78" s="3" customFormat="1" spans="1:14">
+      <c r="AC77" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="78" s="3" customFormat="1" spans="1:29">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -4403,9 +4442,12 @@
       </c>
       <c r="F78" s="10">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="N78" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AC78" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -4475,7 +4517,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" s="3" customFormat="1" spans="1:22">
+    <row r="82" s="3" customFormat="1" spans="1:29">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -4490,7 +4532,7 @@
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="H82" s="11">
         <v>5000</v>
@@ -4505,6 +4547,9 @@
         <v>5000</v>
       </c>
       <c r="V82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AC82" s="11">
         <v>5000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data till 26Jan 8PM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
   <si>
     <t>S.No.</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Ananya Communication-(662161233)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -730,9 +733,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -754,39 +757,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -804,21 +785,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -827,18 +793,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -850,23 +809,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -882,8 +841,45 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,6 +888,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -941,25 +944,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,25 +956,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,7 +998,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,7 +1016,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,91 +1124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,49 +1141,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1209,11 +1171,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1232,12 +1226,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1255,130 +1258,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1761,14 +1764,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AK95"/>
+  <dimension ref="A1:AK98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="Y52" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE15" sqref="AE15"/>
+      <selection pane="bottomRight" activeCell="AF52" sqref="AF52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1905,14 +1908,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>1120100</v>
+        <v>1121100</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>1120100</v>
+        <v>1121100</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -2016,7 +2019,7 @@
       </c>
       <c r="AF2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AG2" s="2">
         <f t="shared" si="0"/>
@@ -3750,7 +3753,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:29">
+    <row r="52" s="3" customFormat="1" spans="1:32">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3765,7 +3768,7 @@
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>19000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -3795,6 +3798,9 @@
         <v>2000</v>
       </c>
       <c r="AC52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AF52" s="11">
         <v>1000</v>
       </c>
     </row>
@@ -4871,6 +4877,11 @@
       </c>
       <c r="AA95" s="11">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="98" spans="31:31">
+      <c r="AE98" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 30Jan 8AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
   <si>
     <t>S.No.</t>
   </si>
@@ -756,11 +756,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -779,46 +779,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -832,9 +795,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -845,6 +807,74 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -863,37 +893,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -903,14 +902,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -918,6 +910,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,19 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,13 +979,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,19 +1003,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,7 +1021,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1045,7 +1051,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1063,6 +1069,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1075,13 +1123,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,61 +1141,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1185,6 +1185,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1196,6 +1205,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1217,6 +1241,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1225,53 +1258,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1281,130 +1281,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1426,7 +1426,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1790,11 +1790,11 @@
   <dimension ref="A1:AK98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AB53" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI10" sqref="AI10"/>
+      <selection pane="bottomRight" activeCell="AI67" sqref="AI67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1931,14 +1931,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F120)</f>
-        <v>1255300</v>
+        <v>1328900</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>1255300</v>
+        <v>1328900</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G120)</f>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="AI2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73600</v>
       </c>
       <c r="AJ2" s="2">
         <f t="shared" si="0"/>
@@ -2125,7 +2125,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="1" spans="1:31">
+    <row r="5" s="3" customFormat="1" spans="1:35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="F5" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>11500</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
@@ -2163,8 +2163,11 @@
       <c r="AE5" s="3">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:30">
+      <c r="AI5" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" spans="1:35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2182,7 +2185,7 @@
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>23000</v>
       </c>
       <c r="H6" s="11">
         <v>3000</v>
@@ -2207,6 +2210,9 @@
       </c>
       <c r="AD6" s="11">
         <v>2000</v>
+      </c>
+      <c r="AI6" s="11">
+        <v>3000</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:34">
@@ -2308,7 +2314,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:31">
+    <row r="10" s="3" customFormat="1" spans="1:35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2323,7 +2329,7 @@
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
-        <v>28000</v>
+        <v>35000</v>
       </c>
       <c r="K10" s="3">
         <v>5000</v>
@@ -2348,6 +2354,9 @@
       </c>
       <c r="AE10" s="3">
         <v>3000</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>7000</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:33">
@@ -2554,7 +2563,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="1" spans="1:33">
+    <row r="15" s="3" customFormat="1" spans="1:35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2570,7 +2579,7 @@
       </c>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="M15" s="3">
         <v>2000</v>
@@ -2587,8 +2596,11 @@
       <c r="AG15" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="AI15" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2606,7 +2618,7 @@
       </c>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
-        <v>2500</v>
+        <v>3300</v>
       </c>
       <c r="H16" s="3">
         <v>500</v>
@@ -2616,6 +2628,9 @@
       </c>
       <c r="Y16" s="3">
         <v>1000</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>800</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1" spans="1:34">
@@ -2852,7 +2867,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" s="3" customFormat="1" spans="1:29">
+    <row r="23" s="3" customFormat="1" spans="1:35">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2870,7 +2885,7 @@
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="P23" s="11">
         <v>3000</v>
@@ -2885,6 +2900,9 @@
         <v>3000</v>
       </c>
       <c r="AC23" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AI23" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -2930,7 +2948,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="1:33">
+    <row r="25" s="3" customFormat="1" spans="1:35">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2945,7 +2963,7 @@
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>27000</v>
+        <v>30000</v>
       </c>
       <c r="H25" s="3">
         <v>3000</v>
@@ -2978,6 +2996,9 @@
         <v>1000</v>
       </c>
       <c r="AG25" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AI25" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3158,7 +3179,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="1" spans="1:29">
+    <row r="31" s="3" customFormat="1" spans="1:35">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -3170,7 +3191,7 @@
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="L31" s="3">
         <v>1000</v>
@@ -3201,6 +3222,9 @@
       </c>
       <c r="AC31" s="3">
         <v>500</v>
+      </c>
+      <c r="AI31" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:28">
@@ -3506,7 +3530,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:33">
+    <row r="41" s="3" customFormat="1" spans="1:35">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3521,7 +3545,7 @@
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>34500</v>
       </c>
       <c r="H41" s="3">
         <v>6000</v>
@@ -3549,6 +3573,9 @@
       </c>
       <c r="AG41" s="3">
         <v>3000</v>
+      </c>
+      <c r="AI41" s="3">
+        <v>4500</v>
       </c>
     </row>
     <row r="42" s="3" customFormat="1" spans="1:34">
@@ -3590,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:31">
+    <row r="44" s="3" customFormat="1" spans="1:35">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3602,7 +3629,7 @@
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="H44" s="3">
         <v>3000</v>
@@ -3626,6 +3653,9 @@
         <v>3000</v>
       </c>
       <c r="AE44" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AI44" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3959,7 +3989,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" s="3" customFormat="1" spans="1:27">
+    <row r="54" s="3" customFormat="1" spans="1:35">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3974,7 +4004,7 @@
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="L54" s="3">
         <v>4000</v>
@@ -3985,8 +4015,11 @@
       <c r="AA54" s="3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="55" s="3" customFormat="1" spans="1:31">
+      <c r="AI54" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="55" s="3" customFormat="1" spans="1:35">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -4001,7 +4034,7 @@
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="H55" s="3">
         <v>5000</v>
@@ -4023,6 +4056,9 @@
       </c>
       <c r="AE55" s="3">
         <v>4500</v>
+      </c>
+      <c r="AI55" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="1" spans="1:33">
@@ -4217,7 +4253,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="62" s="3" customFormat="1" spans="1:30">
+    <row r="62" s="3" customFormat="1" spans="1:35">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -4229,7 +4265,7 @@
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
-        <v>11000</v>
+        <v>14000</v>
       </c>
       <c r="H62" s="3">
         <v>2000</v>
@@ -4248,6 +4284,9 @@
       </c>
       <c r="AD62" s="3">
         <v>1000</v>
+      </c>
+      <c r="AI62" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="63" s="3" customFormat="1" spans="1:29">
@@ -4298,7 +4337,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" s="3" customFormat="1" spans="1:30">
+    <row r="65" s="3" customFormat="1" spans="1:35">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -4310,7 +4349,7 @@
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>45000</v>
+        <v>55000</v>
       </c>
       <c r="H65" s="3">
         <v>5000</v>
@@ -4336,8 +4375,11 @@
       <c r="AD65" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="66" s="3" customFormat="1" spans="1:33">
+      <c r="AI65" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="66" s="3" customFormat="1" spans="1:35">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -4349,7 +4391,7 @@
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
-        <v>24000</v>
+        <v>30000</v>
       </c>
       <c r="H66" s="3">
         <v>3000</v>
@@ -4369,8 +4411,11 @@
       <c r="AG66" s="3">
         <v>3000</v>
       </c>
-    </row>
-    <row r="67" s="3" customFormat="1" spans="1:29">
+      <c r="AI66" s="3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:35">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -4388,7 +4433,7 @@
       </c>
       <c r="F67" s="10">
         <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="J67" s="11">
         <v>4000</v>
@@ -4408,8 +4453,11 @@
       <c r="AC67" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="68" s="3" customFormat="1" spans="1:29">
+      <c r="AI67" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="68" s="3" customFormat="1" spans="1:35">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -4421,13 +4469,16 @@
       </c>
       <c r="F68" s="10">
         <f t="shared" si="3"/>
-        <v>1700</v>
+        <v>2500</v>
       </c>
       <c r="H68" s="3">
         <v>500</v>
       </c>
       <c r="AC68" s="3">
         <v>1200</v>
+      </c>
+      <c r="AI68" s="3">
+        <v>800</v>
       </c>
     </row>
     <row r="69" s="3" customFormat="1" spans="1:34">
@@ -4598,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" s="3" customFormat="1" spans="1:12">
+    <row r="73" s="3" customFormat="1" spans="1:35">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -4616,9 +4667,12 @@
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="L73" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AI73" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -4725,6 +4779,9 @@
       <c r="C79" s="3">
         <v>9852299192</v>
       </c>
+      <c r="D79" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="E79" s="9" t="s">
         <v>133</v>
       </c>
@@ -4793,7 +4850,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="82" s="3" customFormat="1" spans="1:29">
+    <row r="82" s="3" customFormat="1" spans="1:35">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -4808,7 +4865,7 @@
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="H82" s="11">
         <v>5000</v>
@@ -4826,6 +4883,9 @@
         <v>5000</v>
       </c>
       <c r="AC82" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AI82" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -4917,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" s="3" customFormat="1" spans="1:27">
+    <row r="90" s="3" customFormat="1" spans="1:35">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -4932,13 +4992,16 @@
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AA90" s="3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="91" s="3" customFormat="1" spans="1:31">
+      <c r="AI90" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="91" s="3" customFormat="1" spans="1:35">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -4950,12 +5013,15 @@
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="AA91" s="3">
         <v>5000</v>
       </c>
       <c r="AE91" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AI91" s="3">
         <v>5000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data till 31Jan 10AM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="January-2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'January-2021'!$A$1:$AK$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'January-2021'!$A$1:$AK$94</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -207,7 +207,30 @@
         </r>
       </text>
     </comment>
-    <comment ref="U69" authorId="0">
+    <comment ref="AJ54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1244-Cash
+756-Assign New Id Wallet balance remaining</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD69" authorId="0">
+    <comment ref="AD70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH81" authorId="0">
+    <comment ref="AH82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -281,7 +304,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
   <si>
     <t>S.No.</t>
   </si>
@@ -331,6 +354,9 @@
     <t>ARVIND AIRTEL EGRECHARGE CENTR(661591709)</t>
   </si>
   <si>
+    <t>Shakti</t>
+  </si>
+  <si>
     <t>pawan and ravi telicom(660604868)</t>
   </si>
   <si>
@@ -542,6 +568,9 @@
   </si>
   <si>
     <t>DIVYANKA MOBILE CENTER(660315660)</t>
+  </si>
+  <si>
+    <t>Anant Mobile Gallery-(662173660)</t>
   </si>
   <si>
     <t>Neha Phonex(660614432)</t>
@@ -757,10 +786,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -779,19 +808,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -802,8 +822,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -819,48 +908,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -872,7 +923,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -887,29 +938,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -923,18 +952,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -967,7 +996,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,7 +1008,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,19 +1140,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,97 +1158,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,37 +1182,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1164,8 +1199,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1189,7 +1248,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1205,21 +1264,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1241,15 +1285,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1263,13 +1298,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1281,134 +1316,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1426,7 +1461,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1455,6 +1490,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1787,14 +1826,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AK98"/>
+  <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AB53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI67" sqref="AI67"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1930,38 +1969,38 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7">
-        <f>SUM(F3:F120)</f>
-        <v>1328900</v>
+        <f>SUM(F3:F121)</f>
+        <v>1377300</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>1328900</v>
+        <v>1377300</v>
       </c>
       <c r="G2" s="2">
-        <f>SUM(G3:G120)</f>
+        <f>SUM(G3:G121)</f>
         <v>2000</v>
       </c>
       <c r="H2" s="2">
-        <f>SUM(H3:H120)</f>
+        <f>SUM(H3:H121)</f>
         <v>92600</v>
       </c>
       <c r="I2" s="2">
-        <f>SUM(I3:I120)</f>
+        <f>SUM(I3:I121)</f>
         <v>33500</v>
       </c>
       <c r="J2" s="2">
-        <f>SUM(J3:J120)</f>
+        <f>SUM(J3:J121)</f>
         <v>39500</v>
       </c>
       <c r="K2" s="2">
-        <f>SUM(K3:K120)</f>
+        <f>SUM(K3:K121)</f>
         <v>45300</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" ref="L2:AK2" si="0">SUM(L3:L120)</f>
+        <f t="shared" ref="L2:AK2" si="0">SUM(L3:L121)</f>
         <v>53900</v>
       </c>
       <c r="M2" s="2">
@@ -2058,7 +2097,7 @@
       </c>
       <c r="AJ2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48400</v>
       </c>
       <c r="AK2" s="2">
         <f t="shared" si="0"/>
@@ -2215,10 +2254,13 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:34">
+    <row r="7" s="3" customFormat="1" spans="1:36">
       <c r="A7" s="3">
         <v>5</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C7" s="4">
         <v>8210924561</v>
       </c>
@@ -2226,11 +2268,11 @@
         <v>8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>58000</v>
+        <v>65000</v>
       </c>
       <c r="J7" s="11">
         <v>4000</v>
@@ -2258,6 +2300,9 @@
       </c>
       <c r="AH7" s="11">
         <v>8000</v>
+      </c>
+      <c r="AJ7" s="11">
+        <v>7000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:30">
@@ -2271,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
@@ -2298,7 +2343,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
@@ -2325,7 +2370,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
@@ -2364,16 +2409,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4">
         <v>9973022718</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="1"/>
@@ -2400,10 +2445,10 @@
         <v>7004923653</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
@@ -2440,7 +2485,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="1" spans="1:33">
+    <row r="13" s="3" customFormat="1" spans="1:36">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2448,14 +2493,14 @@
         <v>8340182577</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="I13" s="3">
         <v>5000</v>
@@ -2473,6 +2518,9 @@
         <v>5000</v>
       </c>
       <c r="AG13" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AJ13" s="11">
         <v>5000</v>
       </c>
     </row>
@@ -2481,16 +2529,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="4">
         <v>7004740439</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
@@ -2568,14 +2616,14 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
@@ -2605,16 +2653,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4">
         <v>7321004323</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
@@ -2638,16 +2686,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4">
         <v>9608475282</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="10">
         <f t="shared" si="1"/>
@@ -2683,16 +2731,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4">
         <v>9661555592</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="10">
         <f t="shared" si="1"/>
@@ -2719,16 +2767,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4">
         <v>8340523512</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
@@ -2761,10 +2809,10 @@
         <v>8825310472</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
@@ -2789,25 +2837,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="1" spans="1:25">
+    <row r="21" s="3" customFormat="1" spans="1:36">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4">
         <v>7004478123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F21" s="10">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="H21" s="11">
         <v>5000</v>
@@ -2820,6 +2868,9 @@
       </c>
       <c r="Y21" s="11">
         <v>5000</v>
+      </c>
+      <c r="AJ21" s="11">
+        <v>10000</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:34">
@@ -2830,10 +2881,10 @@
         <v>7667895364</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
@@ -2872,16 +2923,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4">
         <v>7006041121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
@@ -2911,16 +2962,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4">
         <v>8709658240</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F24" s="10">
         <f t="shared" si="1"/>
@@ -2956,10 +3007,10 @@
         <v>8709612020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
@@ -3002,7 +3053,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="26" s="3" customFormat="1" spans="1:34">
+    <row r="26" s="3" customFormat="1" spans="1:36">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -3010,14 +3061,14 @@
         <v>9973040600</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="H26" s="3">
         <v>1000</v>
@@ -3047,6 +3098,9 @@
         <v>1000</v>
       </c>
       <c r="AH26" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AJ26" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3058,10 +3112,10 @@
         <v>9973345687</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" si="1"/>
@@ -3085,10 +3139,10 @@
         <v>9631391206</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="1"/>
@@ -3109,13 +3163,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F29" s="10">
         <f t="shared" si="1"/>
@@ -3139,13 +3193,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F30" s="10">
         <f t="shared" si="1"/>
@@ -3184,10 +3238,10 @@
         <v>29</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F31" s="10">
         <f t="shared" si="1"/>
@@ -3227,22 +3281,22 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" s="3" customFormat="1" spans="1:28">
+    <row r="32" s="3" customFormat="1" spans="1:36">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F32" s="10">
         <f t="shared" si="1"/>
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="H32" s="3">
         <v>1000</v>
@@ -3262,20 +3316,23 @@
       <c r="AB32" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="33" s="3" customFormat="1" spans="1:33">
+      <c r="AJ32" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" s="3" customFormat="1" spans="1:36">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="J33" s="3">
         <v>1000</v>
@@ -3290,6 +3347,9 @@
         <v>1000</v>
       </c>
       <c r="AG33" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AJ33" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -3301,10 +3361,10 @@
         <v>7654800030</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F34" s="10">
         <f t="shared" si="1"/>
@@ -3338,19 +3398,19 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:34">
+    <row r="35" s="3" customFormat="1" spans="1:36">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F35" s="10">
-        <f t="shared" ref="F35:F66" si="2">SUM(G35:AK35)</f>
-        <v>30000</v>
+        <f t="shared" ref="F35:F67" si="2">SUM(G35:AK35)</f>
+        <v>33000</v>
       </c>
       <c r="K35" s="11">
         <v>3000</v>
@@ -3379,20 +3439,23 @@
       <c r="AH35" s="11">
         <v>3000</v>
       </c>
-    </row>
-    <row r="36" s="3" customFormat="1" spans="1:33">
+      <c r="AJ35" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="36" s="3" customFormat="1" spans="1:36">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="O36" s="3">
         <v>1000</v>
@@ -3403,23 +3466,26 @@
       <c r="AG36" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="37" s="3" customFormat="1" spans="1:34">
+      <c r="AJ36" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" s="3" customFormat="1" spans="1:36">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" si="2"/>
-        <v>21600</v>
+        <v>24000</v>
       </c>
       <c r="H37" s="11">
         <v>3000</v>
@@ -3441,6 +3507,9 @@
       </c>
       <c r="AH37" s="11">
         <v>3600</v>
+      </c>
+      <c r="AJ37" s="3">
+        <v>2400</v>
       </c>
     </row>
     <row r="38" s="3" customFormat="1" spans="1:29">
@@ -3448,13 +3517,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="2"/>
@@ -3472,10 +3541,10 @@
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F39" s="10">
         <f t="shared" si="2"/>
@@ -3503,19 +3572,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" s="3" customFormat="1" spans="1:31">
+    <row r="40" s="3" customFormat="1" spans="1:36">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F40" s="10">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="H40" s="3">
         <v>2000</v>
@@ -3527,6 +3596,9 @@
         <v>2000</v>
       </c>
       <c r="AE40" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AJ40" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -3538,10 +3610,10 @@
         <v>8210095108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F41" s="10">
         <f t="shared" si="2"/>
@@ -3583,10 +3655,10 @@
         <v>40</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F42" s="10">
         <f t="shared" si="2"/>
@@ -3607,10 +3679,10 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F43" s="10">
         <f t="shared" si="2"/>
@@ -3622,10 +3694,10 @@
         <v>42</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" si="2"/>
@@ -3664,13 +3736,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F45" s="10">
         <f t="shared" si="2"/>
@@ -3695,19 +3767,19 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:31">
+    <row r="46" s="3" customFormat="1" spans="1:36">
       <c r="A46" s="3">
         <v>44</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F46" s="10">
         <f t="shared" si="2"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="I46" s="3">
         <v>3000</v>
@@ -3726,6 +3798,9 @@
       </c>
       <c r="AE46" s="3">
         <v>700</v>
+      </c>
+      <c r="AJ46" s="3">
+        <v>3000</v>
       </c>
     </row>
     <row r="47" s="3" customFormat="1" spans="1:24">
@@ -3733,13 +3808,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F47" s="10">
         <f t="shared" si="2"/>
@@ -3752,25 +3827,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:33">
+    <row r="48" s="3" customFormat="1" spans="1:36">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C48" s="3">
         <v>8863097933</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F48" s="10">
         <f t="shared" si="2"/>
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="L48" s="11">
         <v>6000</v>
@@ -3797,6 +3872,9 @@
         <v>3000</v>
       </c>
       <c r="AG48" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AJ48" s="3">
         <v>3000</v>
       </c>
     </row>
@@ -3805,16 +3883,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" s="3">
         <v>9835443096</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F49" s="10">
         <f t="shared" si="2"/>
@@ -3847,13 +3925,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F50" s="10">
         <f t="shared" si="2"/>
@@ -3877,10 +3955,10 @@
         <v>49</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F51" s="10">
         <f t="shared" si="2"/>
@@ -3898,13 +3976,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
@@ -3947,75 +4025,63 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" s="3" customFormat="1" spans="1:33">
+    <row r="53" s="3" customFormat="1" spans="1:6">
       <c r="A53" s="3">
         <v>51</v>
       </c>
-      <c r="C53" s="3">
-        <v>6202424016</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F53" s="10">
         <f t="shared" si="2"/>
-        <v>17000</v>
-      </c>
-      <c r="J53" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M53" s="11">
-        <v>1000</v>
-      </c>
-      <c r="O53" s="3">
-        <v>1000</v>
-      </c>
-      <c r="Q53" s="3">
-        <v>1000</v>
-      </c>
-      <c r="V53" s="11">
-        <v>2000</v>
-      </c>
-      <c r="Y53" s="11">
-        <v>3000</v>
-      </c>
-      <c r="AC53" s="3">
-        <v>5000</v>
-      </c>
-      <c r="AG53" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="54" s="3" customFormat="1" spans="1:35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" s="3" customFormat="1" spans="1:36">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="C54" s="3">
-        <v>7004211364</v>
+        <v>6202424016</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>89</v>
       </c>
       <c r="F54" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
-      </c>
-      <c r="L54" s="3">
-        <v>4000</v>
-      </c>
-      <c r="U54" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AA54" s="3">
-        <v>4000</v>
-      </c>
-      <c r="AI54" s="3">
+        <v>19000</v>
+      </c>
+      <c r="J54" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M54" s="11">
+        <v>1000</v>
+      </c>
+      <c r="O54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="V54" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Y54" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AC54" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AG54" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AJ54" s="14">
         <v>2000</v>
       </c>
     </row>
@@ -4023,186 +4089,177 @@
       <c r="A55" s="3">
         <v>53</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3">
+        <v>7004211364</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>91</v>
       </c>
       <c r="F55" s="10">
         <f t="shared" si="2"/>
-        <v>40000</v>
-      </c>
-      <c r="H55" s="3">
-        <v>5000</v>
-      </c>
-      <c r="M55" s="11">
-        <v>5000</v>
-      </c>
-      <c r="S55" s="11">
-        <v>5000</v>
+        <v>12000</v>
+      </c>
+      <c r="L55" s="3">
+        <v>4000</v>
       </c>
       <c r="U55" s="3">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="AA55" s="3">
-        <v>5000</v>
-      </c>
-      <c r="AC55" s="3">
-        <v>5500</v>
-      </c>
-      <c r="AE55" s="3">
-        <v>4500</v>
+        <v>4000</v>
       </c>
       <c r="AI55" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="56" s="3" customFormat="1" spans="1:33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="56" s="3" customFormat="1" spans="1:35">
       <c r="A56" s="3">
         <v>54</v>
       </c>
+      <c r="B56" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="D56" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F56" s="10">
         <f t="shared" si="2"/>
-        <v>8000</v>
-      </c>
-      <c r="L56" s="3">
-        <v>2000</v>
+        <v>40000</v>
+      </c>
+      <c r="H56" s="3">
+        <v>5000</v>
+      </c>
+      <c r="M56" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S56" s="11">
+        <v>5000</v>
       </c>
       <c r="U56" s="3">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="AA56" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AG56" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="57" s="3" customFormat="1" spans="1:34">
+        <v>5000</v>
+      </c>
+      <c r="AC56" s="3">
+        <v>5500</v>
+      </c>
+      <c r="AE56" s="3">
+        <v>4500</v>
+      </c>
+      <c r="AI56" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="57" s="3" customFormat="1" spans="1:33">
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="3">
-        <v>9504958065</v>
-      </c>
       <c r="D57" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="F57" s="10">
         <f t="shared" si="2"/>
-        <v>40000</v>
-      </c>
-      <c r="H57" s="11">
-        <v>5000</v>
-      </c>
-      <c r="K57" s="3">
-        <v>5000</v>
-      </c>
-      <c r="N57" s="11">
-        <v>5000</v>
-      </c>
-      <c r="U57" s="11">
-        <v>5000</v>
-      </c>
-      <c r="V57" s="11">
-        <v>5000</v>
-      </c>
-      <c r="AB57" s="3">
-        <v>10000</v>
-      </c>
-      <c r="AH57" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="58" s="3" customFormat="1" spans="1:21">
+        <v>8000</v>
+      </c>
+      <c r="L57" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U57" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AA57" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AG57" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="58" s="3" customFormat="1" spans="1:34">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="3">
+        <v>9504958065</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="E58" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="F58" s="10">
         <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="H58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="K58" s="3">
+        <v>5000</v>
+      </c>
+      <c r="N58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="V58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AB58" s="3">
         <v>10000</v>
       </c>
-      <c r="I58" s="11">
-        <v>5000</v>
-      </c>
-      <c r="U58" s="11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="59" s="3" customFormat="1" spans="1:28">
+      <c r="AH58" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="59" s="3" customFormat="1" spans="1:21">
       <c r="A59" s="3">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="F59" s="10">
         <f t="shared" si="2"/>
-        <v>17000</v>
-      </c>
-      <c r="G59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="K59" s="3">
-        <v>3000</v>
-      </c>
-      <c r="N59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="P59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="S59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="Y59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="AA59" s="11">
-        <v>2000</v>
-      </c>
-      <c r="AB59" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="60" s="3" customFormat="1" spans="1:31">
+        <v>10000</v>
+      </c>
+      <c r="I59" s="11">
+        <v>5000</v>
+      </c>
+      <c r="U59" s="11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="60" s="3" customFormat="1" spans="1:36">
       <c r="A60" s="3">
         <v>58</v>
       </c>
+      <c r="B60" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="D60" s="3" t="s">
         <v>102</v>
       </c>
@@ -4211,22 +4268,37 @@
       </c>
       <c r="F60" s="10">
         <f t="shared" si="2"/>
-        <v>8000</v>
-      </c>
-      <c r="I60" s="3">
-        <v>2000</v>
-      </c>
-      <c r="S60" s="3">
-        <v>2000</v>
-      </c>
-      <c r="X60" s="3">
-        <v>1500</v>
-      </c>
-      <c r="AE60" s="3">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="61" s="3" customFormat="1" spans="1:33">
+        <v>21000</v>
+      </c>
+      <c r="G60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="K60" s="3">
+        <v>3000</v>
+      </c>
+      <c r="N60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="S60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Y60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AA60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AB60" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AJ60" s="11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="61" s="3" customFormat="1" spans="1:31">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -4238,145 +4310,130 @@
       </c>
       <c r="F61" s="10">
         <f t="shared" si="2"/>
-        <v>14000</v>
-      </c>
-      <c r="N61" s="3">
-        <v>4000</v>
-      </c>
-      <c r="U61" s="3">
-        <v>4000</v>
-      </c>
-      <c r="AC61" s="3">
-        <v>4000</v>
-      </c>
-      <c r="AG61" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="62" s="3" customFormat="1" spans="1:35">
+        <v>8000</v>
+      </c>
+      <c r="I61" s="3">
+        <v>2000</v>
+      </c>
+      <c r="S61" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X61" s="3">
+        <v>1500</v>
+      </c>
+      <c r="AE61" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="62" s="3" customFormat="1" spans="1:33">
       <c r="A62" s="3">
         <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F62" s="10">
         <f t="shared" si="2"/>
         <v>14000</v>
       </c>
-      <c r="H62" s="3">
-        <v>2000</v>
-      </c>
-      <c r="L62" s="3">
-        <v>2000</v>
-      </c>
-      <c r="Q62" s="3">
-        <v>2000</v>
+      <c r="N62" s="3">
+        <v>4000</v>
       </c>
       <c r="U62" s="3">
-        <v>2000</v>
-      </c>
-      <c r="X62" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AD62" s="3">
-        <v>1000</v>
-      </c>
-      <c r="AI62" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="63" s="3" customFormat="1" spans="1:29">
+        <v>4000</v>
+      </c>
+      <c r="AC62" s="3">
+        <v>4000</v>
+      </c>
+      <c r="AG62" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="63" s="3" customFormat="1" spans="1:35">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F63" s="10">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>14000</v>
+      </c>
+      <c r="H63" s="3">
+        <v>2000</v>
       </c>
       <c r="L63" s="3">
         <v>2000</v>
       </c>
+      <c r="Q63" s="3">
+        <v>2000</v>
+      </c>
       <c r="U63" s="3">
         <v>2000</v>
       </c>
-      <c r="AC63" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="64" s="3" customFormat="1" spans="1:30">
+      <c r="X63" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AD63" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AI63" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="64" s="3" customFormat="1" spans="1:29">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F64" s="10">
         <f t="shared" si="2"/>
-        <v>3000</v>
-      </c>
-      <c r="N64" s="3">
-        <v>1000</v>
-      </c>
-      <c r="X64" s="3">
-        <v>1000</v>
-      </c>
-      <c r="AD64" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="65" s="3" customFormat="1" spans="1:35">
+        <v>6000</v>
+      </c>
+      <c r="L64" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U64" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AC64" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="65" s="3" customFormat="1" spans="1:30">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F65" s="10">
         <f t="shared" si="2"/>
-        <v>55000</v>
-      </c>
-      <c r="H65" s="3">
-        <v>5000</v>
-      </c>
-      <c r="I65" s="3">
-        <v>5000</v>
-      </c>
-      <c r="L65" s="3">
-        <v>5000</v>
-      </c>
-      <c r="Q65" s="3">
-        <v>10000</v>
-      </c>
-      <c r="U65" s="3">
-        <v>5000</v>
+        <v>3000</v>
+      </c>
+      <c r="N65" s="3">
+        <v>1000</v>
       </c>
       <c r="X65" s="3">
-        <v>5000</v>
-      </c>
-      <c r="AC65" s="3">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="AD65" s="3">
-        <v>5000</v>
-      </c>
-      <c r="AI65" s="3">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="66" s="3" customFormat="1" spans="1:35">
@@ -4384,209 +4441,206 @@
         <v>64</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F66" s="10">
         <f t="shared" si="2"/>
-        <v>30000</v>
+        <v>55000</v>
       </c>
       <c r="H66" s="3">
-        <v>3000</v>
-      </c>
-      <c r="N66" s="3">
-        <v>6000</v>
-      </c>
-      <c r="R66" s="3">
-        <v>3000</v>
-      </c>
-      <c r="U66" s="11">
-        <v>3000</v>
-      </c>
-      <c r="AA66" s="3">
-        <v>6000</v>
-      </c>
-      <c r="AG66" s="3">
-        <v>3000</v>
+        <v>5000</v>
+      </c>
+      <c r="I66" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L66" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Q66" s="3">
+        <v>10000</v>
+      </c>
+      <c r="U66" s="3">
+        <v>5000</v>
+      </c>
+      <c r="X66" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AC66" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AD66" s="3">
+        <v>5000</v>
       </c>
       <c r="AI66" s="3">
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="67" s="3" customFormat="1" spans="1:35">
       <c r="A67" s="3">
         <v>65</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C67" s="3">
-        <v>8825370430</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F67" s="10">
-        <f t="shared" ref="F67:F95" si="3">SUM(G67:AK67)</f>
-        <v>18000</v>
-      </c>
-      <c r="J67" s="11">
-        <v>4000</v>
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+      <c r="H67" s="3">
+        <v>3000</v>
       </c>
       <c r="N67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="R67" s="11">
-        <v>2000</v>
-      </c>
-      <c r="V67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="Y67" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AC67" s="3">
-        <v>2000</v>
+        <v>6000</v>
+      </c>
+      <c r="R67" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U67" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AA67" s="3">
+        <v>6000</v>
+      </c>
+      <c r="AG67" s="3">
+        <v>3000</v>
       </c>
       <c r="AI67" s="3">
-        <v>4000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="68" s="3" customFormat="1" spans="1:35">
       <c r="A68" s="3">
         <v>66</v>
       </c>
+      <c r="B68" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="3">
+        <v>8825370430</v>
+      </c>
       <c r="D68" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F68" s="10">
+        <f t="shared" ref="F68:F96" si="3">SUM(G68:AK68)</f>
+        <v>18000</v>
+      </c>
+      <c r="J68" s="11">
+        <v>4000</v>
+      </c>
+      <c r="N68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="R68" s="11">
+        <v>2000</v>
+      </c>
+      <c r="V68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="Y68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AC68" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AI68" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="1" spans="1:35">
+      <c r="A69" s="3">
+        <v>67</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F69" s="10">
         <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="H68" s="3">
+      <c r="H69" s="3">
         <v>500</v>
       </c>
-      <c r="AC68" s="3">
+      <c r="AC69" s="3">
         <v>1200</v>
       </c>
-      <c r="AI68" s="3">
+      <c r="AI69" s="3">
         <v>800</v>
       </c>
     </row>
-    <row r="69" s="3" customFormat="1" spans="1:34">
-      <c r="A69" s="3">
-        <v>67</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="3">
+    <row r="70" s="3" customFormat="1" spans="1:34">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="3">
         <v>6200769032</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F69" s="10">
+      <c r="D70" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F70" s="10">
         <f t="shared" si="3"/>
         <v>15500</v>
       </c>
-      <c r="H69" s="3">
+      <c r="H70" s="3">
         <v>2800</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K70" s="3">
         <v>1300</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L70" s="3">
         <v>400</v>
       </c>
-      <c r="O69" s="3">
+      <c r="O70" s="3">
         <v>600</v>
       </c>
-      <c r="Q69" s="3">
+      <c r="Q70" s="3">
         <v>500</v>
       </c>
-      <c r="U69" s="11">
+      <c r="U70" s="11">
         <v>2100</v>
       </c>
-      <c r="X69" s="3">
+      <c r="X70" s="3">
         <v>1200</v>
       </c>
-      <c r="Y69" s="3">
+      <c r="Y70" s="3">
         <v>1500</v>
       </c>
-      <c r="AA69" s="3">
-        <v>1000</v>
-      </c>
-      <c r="AD69" s="11">
-        <v>1000</v>
-      </c>
-      <c r="AE69" s="3">
-        <v>1000</v>
-      </c>
-      <c r="AG69" s="3">
+      <c r="AA70" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AD70" s="11">
+        <v>1000</v>
+      </c>
+      <c r="AE70" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AG70" s="3">
         <v>1500</v>
       </c>
-      <c r="AH69" s="3">
+      <c r="AH70" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="70" s="3" customFormat="1" spans="1:33">
-      <c r="A70" s="3">
-        <v>68</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F70" s="10">
-        <f t="shared" si="3"/>
-        <v>27000</v>
-      </c>
-      <c r="I70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="L70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="O70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="R70" s="11">
-        <v>3000</v>
-      </c>
-      <c r="U70" s="11">
-        <v>3000</v>
-      </c>
-      <c r="X70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="Z70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="AC70" s="3">
-        <v>3000</v>
-      </c>
-      <c r="AG70" s="11">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="71" s="3" customFormat="1" spans="1:34">
+    <row r="71" s="3" customFormat="1" spans="1:36">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -4594,232 +4648,250 @@
         <v>119</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F71" s="10">
         <f t="shared" si="3"/>
-        <v>23000</v>
-      </c>
-      <c r="H71" s="3">
-        <v>2000</v>
+        <v>30000</v>
+      </c>
+      <c r="I71" s="3">
+        <v>3000</v>
       </c>
       <c r="L71" s="3">
-        <v>2000</v>
-      </c>
-      <c r="N71" s="11">
-        <v>2000</v>
-      </c>
-      <c r="Q71" s="11">
-        <v>2000</v>
-      </c>
-      <c r="S71" s="3">
-        <v>2000</v>
-      </c>
-      <c r="U71" s="3">
-        <v>2000</v>
-      </c>
-      <c r="X71" s="11">
-        <v>2000</v>
-      </c>
-      <c r="Z71" s="11">
-        <v>3000</v>
-      </c>
-      <c r="AB71" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AG71" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AH71" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="72" s="3" customFormat="1" spans="1:6">
+        <v>3000</v>
+      </c>
+      <c r="O71" s="3">
+        <v>3000</v>
+      </c>
+      <c r="R71" s="11">
+        <v>3000</v>
+      </c>
+      <c r="U71" s="11">
+        <v>3000</v>
+      </c>
+      <c r="X71" s="3">
+        <v>3000</v>
+      </c>
+      <c r="Z71" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AC71" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AG71" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AJ71" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="72" s="3" customFormat="1" spans="1:34">
       <c r="A72" s="3">
         <v>70</v>
       </c>
+      <c r="B72" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="E72" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F72" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" s="3" customFormat="1" spans="1:35">
+        <v>23000</v>
+      </c>
+      <c r="H72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="N72" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Q72" s="11">
+        <v>2000</v>
+      </c>
+      <c r="S72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X72" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Z72" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AB72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AG72" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AH72" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="73" s="3" customFormat="1" spans="1:6">
       <c r="A73" s="3">
         <v>71</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C73" s="13" t="s">
+      <c r="E73" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
-        <v>6000</v>
-      </c>
-      <c r="L73" s="11">
-        <v>3000</v>
-      </c>
-      <c r="AI73" s="11">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="74" s="3" customFormat="1" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" s="3" customFormat="1" spans="1:35">
       <c r="A74" s="3">
         <v>72</v>
       </c>
+      <c r="B74" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E74" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F74" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" s="3" customFormat="1" spans="1:33">
+        <v>6000</v>
+      </c>
+      <c r="L74" s="11">
+        <v>3000</v>
+      </c>
+      <c r="AI74" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="75" s="3" customFormat="1" spans="1:6">
       <c r="A75" s="3">
         <v>73</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E75" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F75" s="10">
         <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-      <c r="M75" s="11">
-        <v>2000</v>
-      </c>
-      <c r="U75" s="3">
-        <v>2000</v>
-      </c>
-      <c r="AG75" s="11">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="76" s="3" customFormat="1" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" s="3" customFormat="1" spans="1:33">
       <c r="A76" s="3">
         <v>74</v>
       </c>
+      <c r="D76" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="E76" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F76" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" s="3" customFormat="1" spans="1:29">
+        <v>8000</v>
+      </c>
+      <c r="M76" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U76" s="3">
+        <v>2000</v>
+      </c>
+      <c r="AG76" s="11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="77" s="3" customFormat="1" spans="1:6">
       <c r="A77" s="3">
         <v>75</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C77" s="3">
-        <v>7004210181</v>
-      </c>
       <c r="E77" s="9" t="s">
         <v>131</v>
       </c>
       <c r="F77" s="10">
         <f t="shared" si="3"/>
-        <v>6000</v>
-      </c>
-      <c r="L77" s="11">
-        <v>2000</v>
-      </c>
-      <c r="V77" s="11">
-        <v>2000</v>
-      </c>
-      <c r="AC77" s="11">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" s="3" customFormat="1" spans="1:29">
       <c r="A78" s="3">
         <v>76</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>73</v>
+      <c r="B78" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="3">
+        <v>7004210181</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F78" s="10">
         <f t="shared" si="3"/>
-        <v>4000</v>
-      </c>
-      <c r="N78" s="11">
-        <v>2000</v>
-      </c>
-      <c r="AC78" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="79" s="3" customFormat="1" spans="1:34">
+        <v>6000</v>
+      </c>
+      <c r="L78" s="11">
+        <v>2000</v>
+      </c>
+      <c r="V78" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AC78" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="79" s="3" customFormat="1" spans="1:29">
       <c r="A79" s="3">
         <v>77</v>
       </c>
-      <c r="C79" s="3">
-        <v>9852299192</v>
-      </c>
       <c r="D79" s="3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F79" s="10">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="AH79" s="3">
-        <v>4000</v>
+      <c r="N79" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AC79" s="3">
+        <v>2000</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="1" spans="1:34">
       <c r="A80" s="3">
         <v>78</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>134</v>
+      <c r="C80" s="3">
+        <v>9852299192</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>135</v>
       </c>
       <c r="F80" s="10">
         <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-      <c r="S80" s="11">
-        <v>2000</v>
-      </c>
-      <c r="U80" s="11">
-        <v>1000</v>
-      </c>
-      <c r="X80" s="11">
-        <v>1000</v>
-      </c>
-      <c r="AH80" s="11">
+        <v>4000</v>
+      </c>
+      <c r="AH80" s="3">
         <v>4000</v>
       </c>
     </row>
@@ -4827,8 +4899,11 @@
       <c r="A81" s="3">
         <v>79</v>
       </c>
+      <c r="B81" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="D81" s="3" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E81" s="9" t="s">
         <v>137</v>
@@ -4837,68 +4912,83 @@
         <f t="shared" si="3"/>
         <v>8000</v>
       </c>
-      <c r="K81" s="3">
-        <v>2000</v>
-      </c>
-      <c r="V81" s="3">
-        <v>3000</v>
-      </c>
-      <c r="AB81" s="3">
+      <c r="S81" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U81" s="11">
+        <v>1000</v>
+      </c>
+      <c r="X81" s="11">
         <v>1000</v>
       </c>
       <c r="AH81" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="82" s="3" customFormat="1" spans="1:35">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="82" s="3" customFormat="1" spans="1:34">
       <c r="A82" s="3">
         <v>80</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="E82" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="F82" s="10">
         <f t="shared" si="3"/>
-        <v>35000</v>
-      </c>
-      <c r="H82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="K82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="P82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="S82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="V82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="AC82" s="11">
-        <v>5000</v>
-      </c>
-      <c r="AI82" s="11">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="83" s="3" customFormat="1" spans="1:6">
+        <v>8000</v>
+      </c>
+      <c r="K82" s="3">
+        <v>2000</v>
+      </c>
+      <c r="V82" s="3">
+        <v>3000</v>
+      </c>
+      <c r="AB82" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AH82" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="83" s="3" customFormat="1" spans="1:35">
       <c r="A83" s="3">
         <v>81</v>
       </c>
+      <c r="B83" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="E83" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F83" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>35000</v>
+      </c>
+      <c r="H83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="K83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="P83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="S83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="V83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AC83" s="11">
+        <v>5000</v>
+      </c>
+      <c r="AI83" s="11">
+        <v>5000</v>
       </c>
     </row>
     <row r="84" s="3" customFormat="1" spans="1:6">
@@ -4906,7 +4996,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F84" s="10">
         <f t="shared" si="3"/>
@@ -4917,9 +5007,8 @@
       <c r="A85" s="3">
         <v>83</v>
       </c>
-      <c r="C85" s="13"/>
       <c r="E85" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F85" s="10">
         <f t="shared" si="3"/>
@@ -4930,8 +5019,9 @@
       <c r="A86" s="3">
         <v>84</v>
       </c>
+      <c r="C86" s="13"/>
       <c r="E86" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F86" s="10">
         <f t="shared" si="3"/>
@@ -4942,11 +5032,8 @@
       <c r="A87" s="3">
         <v>85</v>
       </c>
-      <c r="C87" s="3">
-        <v>9015378357</v>
-      </c>
       <c r="E87" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F87" s="10">
         <f t="shared" si="3"/>
@@ -4957,8 +5044,11 @@
       <c r="A88" s="3">
         <v>86</v>
       </c>
+      <c r="C88" s="3">
+        <v>9015378357</v>
+      </c>
       <c r="E88" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F88" s="10">
         <f t="shared" si="3"/>
@@ -4970,142 +5060,154 @@
         <v>87</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F89" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" s="3" customFormat="1" spans="1:35">
+    <row r="90" s="3" customFormat="1" spans="1:6">
       <c r="A90" s="3">
         <v>88</v>
       </c>
-      <c r="C90" s="3">
-        <v>9934079439</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="E90" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F90" s="10">
         <f t="shared" si="3"/>
-        <v>6000</v>
-      </c>
-      <c r="AA90" s="3">
-        <v>5000</v>
-      </c>
-      <c r="AI90" s="3">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" s="3" customFormat="1" spans="1:35">
       <c r="A91" s="3">
         <v>89</v>
       </c>
+      <c r="C91" s="3">
+        <v>9934079439</v>
+      </c>
       <c r="D91" s="3" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F91" s="10">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>6000</v>
       </c>
       <c r="AA91" s="3">
         <v>5000</v>
       </c>
-      <c r="AE91" s="3">
-        <v>5000</v>
-      </c>
       <c r="AI91" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="92" s="3" customFormat="1" spans="1:6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="92" s="3" customFormat="1" spans="1:35">
       <c r="A92" s="3">
         <v>90</v>
       </c>
-      <c r="C92" s="3">
-        <v>9631378928</v>
-      </c>
       <c r="D92" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F92" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15000</v>
+      </c>
+      <c r="AA92" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AE92" s="3">
+        <v>5000</v>
+      </c>
+      <c r="AI92" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="93" s="3" customFormat="1" spans="1:6">
       <c r="A93" s="3">
         <v>91</v>
       </c>
+      <c r="C93" s="3">
+        <v>9631378928</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="E93" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F93" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" s="3" customFormat="1" spans="1:6">
       <c r="A94" s="3">
         <v>92</v>
       </c>
-      <c r="E94" s="14" t="s">
-        <v>152</v>
+      <c r="E94" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="F94" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:34">
+    <row r="95" spans="1:6">
       <c r="A95" s="3">
         <v>93</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C95" s="3">
-        <v>7004399486</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="15" t="s">
         <v>154</v>
       </c>
       <c r="F95" s="10">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="3">
+        <v>7004399486</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F96" s="10">
+        <f t="shared" si="3"/>
         <v>9000</v>
       </c>
-      <c r="K95" s="11">
-        <v>2000</v>
-      </c>
-      <c r="P95" s="11">
-        <v>2000</v>
-      </c>
-      <c r="W95" s="11">
-        <v>1000</v>
-      </c>
-      <c r="AA95" s="11">
-        <v>2000</v>
-      </c>
-      <c r="AH95" s="11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="98" spans="31:31">
-      <c r="AE98" s="3" t="s">
-        <v>155</v>
+      <c r="K96" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P96" s="11">
+        <v>2000</v>
+      </c>
+      <c r="W96" s="11">
+        <v>1000</v>
+      </c>
+      <c r="AA96" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AH96" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="99" spans="31:31">
+      <c r="AE99" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 31Jan 10PM
</commit_message>
<xml_diff>
--- a/Daily Collection/January-2021-Collection.xlsx
+++ b/Daily Collection/January-2021-Collection.xlsx
@@ -785,10 +785,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -808,8 +808,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -822,16 +830,55 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -839,7 +886,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -854,7 +901,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -869,8 +916,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -885,53 +939,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,19 +953,11 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -1002,7 +1002,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,85 +1050,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,7 +1068,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1122,25 +1146,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,37 +1176,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1193,78 +1193,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1293,153 +1221,225 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1829,11 +1829,11 @@
   <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AI33" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="AK38" sqref="AK38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1970,14 +1970,14 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>SUM(F3:F121)</f>
-        <v>1377300</v>
+        <v>1379300</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7">
         <f>SUM(G2:AK2)</f>
-        <v>1377300</v>
+        <v>1379300</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G121)</f>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="AK2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:27">
@@ -2254,7 +2254,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:36">
+    <row r="7" s="3" customFormat="1" spans="1:37">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>65000</v>
+        <v>66000</v>
       </c>
       <c r="J7" s="11">
         <v>4000</v>
@@ -2303,6 +2303,9 @@
       </c>
       <c r="AJ7" s="11">
         <v>7000</v>
+      </c>
+      <c r="AK7" s="11">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:30">
@@ -3971,7 +3974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" s="3" customFormat="1" spans="1:33">
+    <row r="52" s="3" customFormat="1" spans="1:37">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3986,7 +3989,7 @@
       </c>
       <c r="F52" s="10">
         <f t="shared" si="2"/>
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="H52" s="11">
         <v>3000</v>
@@ -4022,6 +4025,9 @@
         <v>1000</v>
       </c>
       <c r="AG52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AK52" s="11">
         <v>1000</v>
       </c>
     </row>

</xml_diff>